<commit_message>
!U updated docs and Maya release codes
</commit_message>
<xml_diff>
--- a/Codebase_Tracker.xlsx
+++ b/Codebase_Tracker.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ProPack" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="227">
   <si>
     <t>Module</t>
   </si>
@@ -658,6 +658,45 @@
   </si>
   <si>
     <t>This is now patched, fixing issues in some of the fk&gt;ik sytem calls (seen primarily on the Puppet rigs head system)</t>
+  </si>
+  <si>
+    <t>parallel support</t>
+  </si>
+  <si>
+    <t>playback_performance, parallel_eval_freeze, parallel_eval_unfreeze_all</t>
+  </si>
+  <si>
+    <t>wrap over the eval Manager 'frozen' node state to stop node evaluating in parallel mode and added performance tester</t>
+  </si>
+  <si>
+    <t>Used to speed up rigs under certain cases and performance test</t>
+  </si>
+  <si>
+    <t>Maya Units</t>
+  </si>
+  <si>
+    <t>The API load code wasn't dealing with unit conversion so units in meters were being loaded in centimeters.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">parallel_eval_mute/reset </t>
+  </si>
+  <si>
+    <t>new management for parallel eval optimisations</t>
+  </si>
+  <si>
+    <t>This sets the frozen attr state on all nodes returned by the parallel_eval_get_nodes fun, designed to be overloaded as needed.</t>
+  </si>
+  <si>
+    <t>Handling added for all unikt conversions, this uses the sceneUnits stored in the file to convert all linear units.</t>
+  </si>
+  <si>
+    <t>DataMap</t>
+  </si>
+  <si>
+    <t>The  load code wasn't dealing with unit conversion, if a pose had been saved in a scene when it was centimeters, buth the scene units had been changed then the pose would fail to load correctly</t>
+  </si>
+  <si>
+    <t>Handling added for all unit conversions, this uses the sceneUnits stored in the file to convert all linear units.</t>
   </si>
 </sst>
 </file>
@@ -845,7 +884,7 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="103">
+  <cellXfs count="108">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1149,6 +1188,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="2" xfId="4" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1466,10 +1520,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:M56"/>
+  <dimension ref="A2:M59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="I36" sqref="I36"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17:XFD17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1479,7 +1533,7 @@
     <col min="4" max="4" width="20.7109375" style="5" customWidth="1"/>
     <col min="5" max="5" width="12.28515625" style="16" customWidth="1"/>
     <col min="6" max="6" width="12.28515625" style="9" customWidth="1"/>
-    <col min="7" max="7" width="24.7109375" style="5" customWidth="1"/>
+    <col min="7" max="7" width="29.140625" style="5" customWidth="1"/>
     <col min="8" max="8" width="60.28515625" style="5" customWidth="1"/>
     <col min="9" max="9" width="62.7109375" style="5" customWidth="1"/>
     <col min="10" max="10" width="17" style="64" customWidth="1"/>
@@ -1488,17 +1542,17 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:13" ht="21">
-      <c r="B2" s="102" t="s">
+      <c r="B2" s="107" t="s">
         <v>137</v>
       </c>
-      <c r="C2" s="102"/>
-      <c r="D2" s="102"/>
-      <c r="E2" s="102"/>
-      <c r="F2" s="102"/>
-      <c r="G2" s="102"/>
-      <c r="H2" s="102"/>
-      <c r="I2" s="102"/>
-      <c r="J2" s="102"/>
+      <c r="C2" s="107"/>
+      <c r="D2" s="107"/>
+      <c r="E2" s="107"/>
+      <c r="F2" s="107"/>
+      <c r="G2" s="107"/>
+      <c r="H2" s="107"/>
+      <c r="I2" s="107"/>
+      <c r="J2" s="107"/>
     </row>
     <row r="3" spans="1:13" ht="15.6" customHeight="1"/>
     <row r="4" spans="1:13" s="2" customFormat="1" ht="24" customHeight="1">
@@ -1739,8 +1793,8 @@
       <c r="C14" s="49" t="s">
         <v>28</v>
       </c>
-      <c r="D14" s="20" t="s">
-        <v>94</v>
+      <c r="D14" s="101" t="s">
+        <v>5</v>
       </c>
       <c r="E14" s="21">
         <v>42839</v>
@@ -1766,8 +1820,8 @@
       <c r="C15" s="73" t="s">
         <v>28</v>
       </c>
-      <c r="D15" s="74" t="s">
-        <v>94</v>
+      <c r="D15" s="87" t="s">
+        <v>5</v>
       </c>
       <c r="E15" s="75">
         <v>42867</v>
@@ -1786,63 +1840,67 @@
       </c>
       <c r="J15" s="77"/>
     </row>
-    <row r="16" spans="1:13" ht="30" customHeight="1">
-      <c r="C16" s="52"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="11"/>
-    </row>
-    <row r="17" spans="2:10" ht="45">
-      <c r="B17" s="26" t="s">
-        <v>16</v>
-      </c>
-      <c r="C17" s="51" t="s">
-        <v>61</v>
-      </c>
-      <c r="D17" s="27" t="s">
-        <v>62</v>
-      </c>
-      <c r="E17" s="28">
-        <v>42745</v>
-      </c>
-      <c r="F17" s="29" t="s">
+    <row r="16" spans="1:13" ht="45">
+      <c r="B16" s="72" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" s="73" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16" s="87" t="s">
+        <v>214</v>
+      </c>
+      <c r="E16" s="75">
+        <v>42983</v>
+      </c>
+      <c r="F16" s="29" t="s">
         <v>98</v>
       </c>
-      <c r="G17" s="30"/>
-      <c r="H17" s="31" t="s">
-        <v>70</v>
-      </c>
-      <c r="I17" s="27"/>
-      <c r="J17" s="68"/>
-    </row>
-    <row r="18" spans="2:10" ht="45">
-      <c r="B18" s="26" t="s">
-        <v>16</v>
-      </c>
-      <c r="C18" s="51" t="s">
-        <v>61</v>
-      </c>
-      <c r="D18" s="27" t="s">
-        <v>71</v>
-      </c>
-      <c r="E18" s="28">
-        <v>42750</v>
-      </c>
-      <c r="F18" s="29" t="s">
-        <v>98</v>
-      </c>
-      <c r="G18" s="30" t="s">
-        <v>72</v>
-      </c>
-      <c r="H18" s="31" t="s">
-        <v>73</v>
-      </c>
-      <c r="I18" s="31" t="s">
-        <v>74</v>
-      </c>
-      <c r="J18" s="68"/>
-    </row>
-    <row r="19" spans="2:10" ht="60">
+      <c r="G16" s="102" t="s">
+        <v>215</v>
+      </c>
+      <c r="H16" s="78" t="s">
+        <v>216</v>
+      </c>
+      <c r="I16" s="78" t="s">
+        <v>217</v>
+      </c>
+      <c r="J16" s="77"/>
+    </row>
+    <row r="17" spans="2:10" ht="30">
+      <c r="B17" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" s="49" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17" s="101" t="s">
+        <v>5</v>
+      </c>
+      <c r="E17" s="21">
+        <v>42996</v>
+      </c>
+      <c r="F17" s="93" t="s">
+        <v>107</v>
+      </c>
+      <c r="G17" s="106" t="s">
+        <v>218</v>
+      </c>
+      <c r="H17" s="71" t="s">
+        <v>219</v>
+      </c>
+      <c r="I17" s="71" t="s">
+        <v>223</v>
+      </c>
+      <c r="J17" s="67"/>
+    </row>
+    <row r="18" spans="2:10" ht="30" customHeight="1">
+      <c r="C18" s="52"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="11"/>
+    </row>
+    <row r="19" spans="2:10" ht="45">
       <c r="B19" s="26" t="s">
         <v>16</v>
       </c>
@@ -1850,160 +1908,160 @@
         <v>61</v>
       </c>
       <c r="D19" s="27" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="E19" s="28">
-        <v>42860</v>
+        <v>42745</v>
       </c>
       <c r="F19" s="29" t="s">
         <v>98</v>
       </c>
-      <c r="G19" s="30" t="s">
+      <c r="G19" s="30"/>
+      <c r="H19" s="31" t="s">
+        <v>70</v>
+      </c>
+      <c r="I19" s="27"/>
+      <c r="J19" s="68"/>
+    </row>
+    <row r="20" spans="2:10" ht="45">
+      <c r="B20" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="C20" s="51" t="s">
+        <v>61</v>
+      </c>
+      <c r="D20" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="E20" s="28">
+        <v>42750</v>
+      </c>
+      <c r="F20" s="29" t="s">
+        <v>98</v>
+      </c>
+      <c r="G20" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="H20" s="31" t="s">
+        <v>73</v>
+      </c>
+      <c r="I20" s="31" t="s">
+        <v>74</v>
+      </c>
+      <c r="J20" s="68"/>
+    </row>
+    <row r="21" spans="2:10" ht="60">
+      <c r="B21" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="C21" s="51" t="s">
+        <v>61</v>
+      </c>
+      <c r="D21" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="E21" s="28">
+        <v>42860</v>
+      </c>
+      <c r="F21" s="29" t="s">
+        <v>98</v>
+      </c>
+      <c r="G21" s="30" t="s">
         <v>191</v>
       </c>
-      <c r="H19" s="31" t="s">
+      <c r="H21" s="31" t="s">
         <v>192</v>
       </c>
-      <c r="I19" s="31" t="s">
+      <c r="I21" s="31" t="s">
         <v>193</v>
       </c>
-      <c r="J19" s="68"/>
-    </row>
-    <row r="20" spans="2:10" ht="30" customHeight="1">
-      <c r="B20"/>
-      <c r="C20" s="53"/>
-      <c r="D20"/>
-      <c r="E20"/>
-      <c r="F20"/>
-      <c r="G20"/>
-      <c r="H20"/>
-      <c r="I20"/>
-      <c r="J20" s="65"/>
-    </row>
-    <row r="21" spans="2:10" ht="45">
-      <c r="B21" s="34" t="s">
-        <v>16</v>
-      </c>
-      <c r="C21" s="50" t="s">
+      <c r="J21" s="68"/>
+    </row>
+    <row r="22" spans="2:10" ht="30" customHeight="1">
+      <c r="B22"/>
+      <c r="C22" s="53"/>
+      <c r="D22"/>
+      <c r="E22"/>
+      <c r="F22"/>
+      <c r="G22"/>
+      <c r="H22"/>
+      <c r="I22"/>
+      <c r="J22" s="65"/>
+    </row>
+    <row r="23" spans="2:10" ht="45">
+      <c r="B23" s="34" t="s">
+        <v>16</v>
+      </c>
+      <c r="C23" s="50" t="s">
         <v>19</v>
       </c>
-      <c r="D21" s="35" t="s">
+      <c r="D23" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="E21" s="36"/>
-      <c r="F21" s="37" t="s">
+      <c r="E23" s="36"/>
+      <c r="F23" s="37" t="s">
         <v>97</v>
       </c>
-      <c r="G21" s="35"/>
-      <c r="H21" s="38" t="s">
+      <c r="G23" s="35"/>
+      <c r="H23" s="38" t="s">
         <v>22</v>
       </c>
-      <c r="I21" s="35" t="s">
+      <c r="I23" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="J21" s="66"/>
-    </row>
-    <row r="22" spans="2:10" ht="60">
-      <c r="B22" s="26" t="s">
-        <v>16</v>
-      </c>
-      <c r="C22" s="51" t="s">
+      <c r="J23" s="66"/>
+    </row>
+    <row r="24" spans="2:10" ht="60">
+      <c r="B24" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="C24" s="51" t="s">
         <v>19</v>
       </c>
-      <c r="D22" s="27" t="s">
+      <c r="D24" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="E22" s="28">
+      <c r="E24" s="28">
         <v>42724</v>
       </c>
-      <c r="F22" s="29" t="s">
+      <c r="F24" s="29" t="s">
         <v>98</v>
       </c>
-      <c r="G22" s="30"/>
-      <c r="H22" s="31" t="s">
+      <c r="G24" s="30"/>
+      <c r="H24" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="I22" s="27"/>
-      <c r="J22" s="68"/>
-    </row>
-    <row r="23" spans="2:10" ht="45">
-      <c r="B23" s="26" t="s">
-        <v>16</v>
-      </c>
-      <c r="C23" s="51" t="s">
+      <c r="I24" s="27"/>
+      <c r="J24" s="68"/>
+    </row>
+    <row r="25" spans="2:10" ht="45">
+      <c r="B25" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="C25" s="51" t="s">
         <v>19</v>
       </c>
-      <c r="D23" s="27" t="s">
+      <c r="D25" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="E23" s="28">
+      <c r="E25" s="28">
         <v>42802</v>
-      </c>
-      <c r="F23" s="29" t="s">
-        <v>98</v>
-      </c>
-      <c r="G23" s="30"/>
-      <c r="H23" s="31" t="s">
-        <v>147</v>
-      </c>
-      <c r="I23" s="27"/>
-      <c r="J23" s="68"/>
-    </row>
-    <row r="24" spans="2:10" ht="30" customHeight="1">
-      <c r="C24" s="52"/>
-      <c r="F24" s="6"/>
-      <c r="G24" s="7"/>
-      <c r="H24" s="11"/>
-    </row>
-    <row r="25" spans="2:10" ht="15.75">
-      <c r="B25" s="26" t="s">
-        <v>16</v>
-      </c>
-      <c r="C25" s="51" t="s">
-        <v>17</v>
-      </c>
-      <c r="D25" s="27" t="s">
-        <v>40</v>
-      </c>
-      <c r="E25" s="28">
-        <v>42720</v>
       </c>
       <c r="F25" s="29" t="s">
         <v>98</v>
       </c>
-      <c r="G25" s="30" t="s">
-        <v>52</v>
-      </c>
+      <c r="G25" s="30"/>
       <c r="H25" s="31" t="s">
-        <v>31</v>
+        <v>147</v>
       </c>
       <c r="I25" s="27"/>
       <c r="J25" s="68"/>
     </row>
-    <row r="26" spans="2:10" ht="30">
-      <c r="B26" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="C26" s="49" t="s">
-        <v>17</v>
-      </c>
-      <c r="D26" s="20" t="s">
-        <v>41</v>
-      </c>
-      <c r="E26" s="21">
-        <v>42724</v>
-      </c>
-      <c r="F26" s="22" t="s">
-        <v>107</v>
-      </c>
-      <c r="G26" s="23" t="s">
-        <v>49</v>
-      </c>
-      <c r="H26" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="I26" s="20"/>
-      <c r="J26" s="67"/>
+    <row r="26" spans="2:10" ht="30" customHeight="1">
+      <c r="C26" s="52"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="7"/>
+      <c r="H26" s="11"/>
     </row>
     <row r="27" spans="2:10" ht="15.75">
       <c r="B27" s="26" t="s">
@@ -2013,51 +2071,47 @@
         <v>17</v>
       </c>
       <c r="D27" s="27" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E27" s="28">
-        <v>42726</v>
+        <v>42720</v>
       </c>
       <c r="F27" s="29" t="s">
         <v>98</v>
       </c>
       <c r="G27" s="30" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="H27" s="31" t="s">
-        <v>77</v>
+        <v>31</v>
       </c>
       <c r="I27" s="27"/>
       <c r="J27" s="68"/>
     </row>
     <row r="28" spans="2:10" ht="30">
-      <c r="B28" s="26" t="s">
-        <v>16</v>
-      </c>
-      <c r="C28" s="51" t="s">
+      <c r="B28" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="C28" s="49" t="s">
         <v>17</v>
       </c>
-      <c r="D28" s="27" t="s">
-        <v>42</v>
-      </c>
-      <c r="E28" s="28">
-        <v>42726</v>
-      </c>
-      <c r="F28" s="29" t="s">
-        <v>98</v>
-      </c>
-      <c r="G28" s="30" t="s">
-        <v>48</v>
-      </c>
-      <c r="H28" s="31" t="s">
-        <v>76</v>
-      </c>
-      <c r="I28" s="31" t="s">
-        <v>36</v>
-      </c>
-      <c r="J28" s="68" t="s">
-        <v>139</v>
-      </c>
+      <c r="D28" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="E28" s="21">
+        <v>42724</v>
+      </c>
+      <c r="F28" s="22" t="s">
+        <v>107</v>
+      </c>
+      <c r="G28" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="H28" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="I28" s="20"/>
+      <c r="J28" s="67"/>
     </row>
     <row r="29" spans="2:10" ht="15.75">
       <c r="B29" s="26" t="s">
@@ -2079,41 +2133,41 @@
         <v>48</v>
       </c>
       <c r="H29" s="31" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I29" s="27"/>
       <c r="J29" s="68"/>
     </row>
-    <row r="30" spans="2:10" ht="45">
-      <c r="B30" s="34" t="s">
-        <v>16</v>
-      </c>
-      <c r="C30" s="50" t="s">
+    <row r="30" spans="2:10" ht="30">
+      <c r="B30" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="C30" s="51" t="s">
         <v>17</v>
       </c>
-      <c r="D30" s="35" t="s">
-        <v>41</v>
-      </c>
-      <c r="E30" s="36">
-        <v>42732</v>
-      </c>
-      <c r="F30" s="37" t="s">
-        <v>97</v>
-      </c>
-      <c r="G30" s="40" t="s">
-        <v>51</v>
-      </c>
-      <c r="H30" s="38" t="s">
-        <v>43</v>
-      </c>
-      <c r="I30" s="38" t="s">
-        <v>45</v>
-      </c>
-      <c r="J30" s="66" t="s">
+      <c r="D30" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="E30" s="28">
+        <v>42726</v>
+      </c>
+      <c r="F30" s="29" t="s">
+        <v>98</v>
+      </c>
+      <c r="G30" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="H30" s="31" t="s">
+        <v>76</v>
+      </c>
+      <c r="I30" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="J30" s="68" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="31" spans="2:10" ht="45">
+    <row r="31" spans="2:10" ht="15.75">
       <c r="B31" s="26" t="s">
         <v>16</v>
       </c>
@@ -2121,24 +2175,24 @@
         <v>17</v>
       </c>
       <c r="D31" s="27" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E31" s="28">
-        <v>42755</v>
+        <v>42726</v>
       </c>
       <c r="F31" s="29" t="s">
         <v>98</v>
       </c>
       <c r="G31" s="30" t="s">
-        <v>90</v>
+        <v>48</v>
       </c>
       <c r="H31" s="31" t="s">
-        <v>91</v>
-      </c>
-      <c r="I31" s="31"/>
+        <v>78</v>
+      </c>
+      <c r="I31" s="27"/>
       <c r="J31" s="68"/>
     </row>
-    <row r="32" spans="2:10" ht="30">
+    <row r="32" spans="2:10" ht="45">
       <c r="B32" s="34" t="s">
         <v>16</v>
       </c>
@@ -2146,101 +2200,105 @@
         <v>17</v>
       </c>
       <c r="D32" s="35" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E32" s="36">
-        <v>42758</v>
+        <v>42732</v>
       </c>
       <c r="F32" s="37" t="s">
         <v>97</v>
       </c>
       <c r="G32" s="40" t="s">
+        <v>51</v>
+      </c>
+      <c r="H32" s="38" t="s">
+        <v>43</v>
+      </c>
+      <c r="I32" s="38" t="s">
+        <v>45</v>
+      </c>
+      <c r="J32" s="66" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="33" spans="2:10" ht="45">
+      <c r="B33" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="C33" s="51" t="s">
+        <v>17</v>
+      </c>
+      <c r="D33" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="E33" s="28">
+        <v>42755</v>
+      </c>
+      <c r="F33" s="29" t="s">
+        <v>98</v>
+      </c>
+      <c r="G33" s="30" t="s">
+        <v>90</v>
+      </c>
+      <c r="H33" s="31" t="s">
+        <v>91</v>
+      </c>
+      <c r="I33" s="31"/>
+      <c r="J33" s="68"/>
+    </row>
+    <row r="34" spans="2:10" ht="30">
+      <c r="B34" s="34" t="s">
+        <v>16</v>
+      </c>
+      <c r="C34" s="50" t="s">
+        <v>17</v>
+      </c>
+      <c r="D34" s="35" t="s">
+        <v>42</v>
+      </c>
+      <c r="E34" s="36">
+        <v>42758</v>
+      </c>
+      <c r="F34" s="37" t="s">
+        <v>97</v>
+      </c>
+      <c r="G34" s="40" t="s">
         <v>92</v>
       </c>
-      <c r="H32" s="38" t="s">
+      <c r="H34" s="38" t="s">
         <v>93</v>
       </c>
-      <c r="I32" s="38"/>
-      <c r="J32" s="66"/>
-    </row>
-    <row r="33" spans="2:10" ht="75">
-      <c r="B33" s="34" t="s">
-        <v>16</v>
-      </c>
-      <c r="C33" s="50" t="s">
+      <c r="I34" s="38"/>
+      <c r="J34" s="66"/>
+    </row>
+    <row r="35" spans="2:10" ht="75">
+      <c r="B35" s="34" t="s">
+        <v>16</v>
+      </c>
+      <c r="C35" s="50" t="s">
         <v>17</v>
       </c>
-      <c r="D33" s="35" t="s">
+      <c r="D35" s="35" t="s">
         <v>115</v>
       </c>
-      <c r="E33" s="36">
+      <c r="E35" s="36">
         <v>42772</v>
       </c>
-      <c r="F33" s="37" t="s">
+      <c r="F35" s="37" t="s">
         <v>97</v>
       </c>
-      <c r="G33" s="40" t="s">
+      <c r="G35" s="40" t="s">
         <v>112</v>
       </c>
-      <c r="H33" s="38" t="s">
+      <c r="H35" s="38" t="s">
         <v>113</v>
       </c>
-      <c r="I33" s="38" t="s">
+      <c r="I35" s="38" t="s">
         <v>114</v>
       </c>
-      <c r="J33" s="66"/>
-    </row>
-    <row r="34" spans="2:10" ht="45">
-      <c r="B34" s="26" t="s">
-        <v>16</v>
-      </c>
-      <c r="C34" s="51" t="s">
-        <v>17</v>
-      </c>
-      <c r="D34" s="27" t="s">
-        <v>41</v>
-      </c>
-      <c r="E34" s="28">
-        <v>42795</v>
-      </c>
-      <c r="F34" s="29" t="s">
-        <v>98</v>
-      </c>
-      <c r="G34" s="30" t="s">
-        <v>143</v>
-      </c>
-      <c r="H34" s="31" t="s">
-        <v>159</v>
-      </c>
-      <c r="I34" s="31"/>
-      <c r="J34" s="68"/>
-    </row>
-    <row r="35" spans="2:10" ht="15.75">
-      <c r="B35" s="26" t="s">
-        <v>16</v>
-      </c>
-      <c r="C35" s="51" t="s">
-        <v>17</v>
-      </c>
-      <c r="D35" s="27" t="s">
-        <v>41</v>
-      </c>
-      <c r="E35" s="28">
-        <v>42816</v>
-      </c>
-      <c r="F35" s="29" t="s">
-        <v>98</v>
-      </c>
-      <c r="G35" s="30" t="s">
-        <v>158</v>
-      </c>
-      <c r="H35" s="31" t="s">
-        <v>160</v>
-      </c>
-      <c r="I35" s="31"/>
-      <c r="J35" s="68"/>
-    </row>
-    <row r="36" spans="2:10" ht="30">
+      <c r="J35" s="66"/>
+    </row>
+    <row r="36" spans="2:10" ht="45">
       <c r="B36" s="26" t="s">
         <v>16</v>
       </c>
@@ -2251,220 +2309,237 @@
         <v>41</v>
       </c>
       <c r="E36" s="28">
+        <v>42795</v>
+      </c>
+      <c r="F36" s="29" t="s">
+        <v>98</v>
+      </c>
+      <c r="G36" s="30" t="s">
+        <v>143</v>
+      </c>
+      <c r="H36" s="31" t="s">
+        <v>159</v>
+      </c>
+      <c r="I36" s="31"/>
+      <c r="J36" s="68"/>
+    </row>
+    <row r="37" spans="2:10" ht="15.75">
+      <c r="B37" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="C37" s="51" t="s">
+        <v>17</v>
+      </c>
+      <c r="D37" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="E37" s="28">
+        <v>42816</v>
+      </c>
+      <c r="F37" s="29" t="s">
+        <v>98</v>
+      </c>
+      <c r="G37" s="30" t="s">
+        <v>158</v>
+      </c>
+      <c r="H37" s="31" t="s">
+        <v>160</v>
+      </c>
+      <c r="I37" s="31"/>
+      <c r="J37" s="68"/>
+    </row>
+    <row r="38" spans="2:10" ht="30">
+      <c r="B38" s="103" t="s">
+        <v>16</v>
+      </c>
+      <c r="C38" s="49" t="s">
+        <v>17</v>
+      </c>
+      <c r="D38" s="101" t="s">
+        <v>41</v>
+      </c>
+      <c r="E38" s="104">
         <v>42909</v>
       </c>
-      <c r="F36" s="29" t="s">
+      <c r="F38" s="93" t="s">
         <v>107</v>
       </c>
-      <c r="G36" s="30" t="s">
+      <c r="G38" s="91" t="s">
         <v>211</v>
       </c>
-      <c r="H36" s="31" t="s">
+      <c r="H38" s="71" t="s">
         <v>212</v>
       </c>
-      <c r="I36" s="31" t="s">
+      <c r="I38" s="71" t="s">
         <v>213</v>
       </c>
-      <c r="J36" s="68"/>
-    </row>
-    <row r="37" spans="2:10" ht="30" customHeight="1">
-      <c r="C37" s="52"/>
-      <c r="F37" s="6"/>
-      <c r="G37" s="7"/>
-      <c r="H37" s="11"/>
-    </row>
-    <row r="38" spans="2:10" ht="60">
-      <c r="B38" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="C38" s="49" t="s">
+      <c r="J38" s="105"/>
+    </row>
+    <row r="39" spans="2:10" ht="45">
+      <c r="B39" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="C39" s="51" t="s">
+        <v>17</v>
+      </c>
+      <c r="D39" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="E39" s="28">
+        <v>42993</v>
+      </c>
+      <c r="F39" s="29" t="s">
+        <v>98</v>
+      </c>
+      <c r="G39" s="30" t="s">
+        <v>220</v>
+      </c>
+      <c r="H39" s="31" t="s">
+        <v>221</v>
+      </c>
+      <c r="I39" s="31" t="s">
+        <v>222</v>
+      </c>
+      <c r="J39" s="68"/>
+    </row>
+    <row r="40" spans="2:10" ht="30" customHeight="1">
+      <c r="C40" s="52"/>
+      <c r="F40" s="6"/>
+      <c r="G40" s="7"/>
+      <c r="H40" s="11"/>
+    </row>
+    <row r="41" spans="2:10" ht="60">
+      <c r="B41" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="C41" s="49" t="s">
         <v>13</v>
       </c>
-      <c r="D38" s="20" t="s">
+      <c r="D41" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="E38" s="21">
+      <c r="E41" s="21">
         <v>42734</v>
       </c>
-      <c r="F38" s="22" t="s">
+      <c r="F41" s="22" t="s">
         <v>107</v>
       </c>
-      <c r="G38" s="23" t="s">
+      <c r="G41" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="H38" s="24" t="s">
+      <c r="H41" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="I38" s="24" t="s">
+      <c r="I41" s="24" t="s">
         <v>132</v>
       </c>
-      <c r="J38" s="67"/>
-    </row>
-    <row r="39" spans="2:10" ht="45">
-      <c r="B39" s="34" t="s">
-        <v>16</v>
-      </c>
-      <c r="C39" s="50" t="s">
+      <c r="J41" s="67"/>
+    </row>
+    <row r="42" spans="2:10" ht="45">
+      <c r="B42" s="34" t="s">
+        <v>16</v>
+      </c>
+      <c r="C42" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="D39" s="35" t="s">
+      <c r="D42" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="E39" s="36">
+      <c r="E42" s="36">
         <v>42740</v>
       </c>
-      <c r="F39" s="37" t="s">
+      <c r="F42" s="37" t="s">
         <v>97</v>
       </c>
-      <c r="G39" s="40" t="s">
+      <c r="G42" s="40" t="s">
         <v>75</v>
       </c>
-      <c r="H39" s="38" t="s">
+      <c r="H42" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="I39" s="35"/>
-      <c r="J39" s="66"/>
-    </row>
-    <row r="40" spans="2:10" ht="45">
-      <c r="B40" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="C40" s="49" t="s">
+      <c r="I42" s="35"/>
+      <c r="J42" s="66"/>
+    </row>
+    <row r="43" spans="2:10" ht="45">
+      <c r="B43" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="C43" s="49" t="s">
         <v>13</v>
       </c>
-      <c r="D40" s="20" t="s">
+      <c r="D43" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="E40" s="21">
+      <c r="E43" s="21">
         <v>42745</v>
       </c>
-      <c r="F40" s="22" t="s">
+      <c r="F43" s="22" t="s">
         <v>107</v>
       </c>
-      <c r="G40" s="23" t="s">
+      <c r="G43" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="H40" s="24" t="s">
+      <c r="H43" s="24" t="s">
         <v>64</v>
       </c>
-      <c r="I40" s="20" t="s">
+      <c r="I43" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="J40" s="67"/>
-    </row>
-    <row r="41" spans="2:10" ht="45">
-      <c r="B41" s="79" t="s">
-        <v>16</v>
-      </c>
-      <c r="C41" s="80" t="s">
+      <c r="J43" s="67"/>
+    </row>
+    <row r="44" spans="2:10" ht="45">
+      <c r="B44" s="79" t="s">
+        <v>16</v>
+      </c>
+      <c r="C44" s="80" t="s">
         <v>13</v>
       </c>
-      <c r="D41" s="83" t="s">
+      <c r="D44" s="83" t="s">
         <v>13</v>
       </c>
-      <c r="E41" s="81">
+      <c r="E44" s="81">
         <v>42811</v>
       </c>
-      <c r="F41" s="13" t="s">
+      <c r="F44" s="13" t="s">
         <v>136</v>
       </c>
-      <c r="G41" s="46" t="s">
+      <c r="G44" s="46" t="s">
         <v>151</v>
       </c>
-      <c r="H41" s="84" t="s">
+      <c r="H44" s="84" t="s">
         <v>152</v>
       </c>
-      <c r="I41" s="83" t="s">
+      <c r="I44" s="83" t="s">
         <v>153</v>
       </c>
-      <c r="J41" s="82"/>
-    </row>
-    <row r="42" spans="2:10" ht="45">
-      <c r="B42" s="86" t="s">
-        <v>16</v>
-      </c>
-      <c r="C42" s="73" t="s">
+      <c r="J44" s="82"/>
+    </row>
+    <row r="45" spans="2:10" ht="45">
+      <c r="B45" s="86" t="s">
+        <v>16</v>
+      </c>
+      <c r="C45" s="73" t="s">
         <v>13</v>
       </c>
-      <c r="D42" s="87" t="s">
+      <c r="D45" s="87" t="s">
         <v>13</v>
       </c>
-      <c r="E42" s="88">
+      <c r="E45" s="88">
         <v>42817</v>
       </c>
-      <c r="F42" s="89" t="s">
+      <c r="F45" s="89" t="s">
         <v>98</v>
       </c>
-      <c r="G42" s="30" t="s">
+      <c r="G45" s="30" t="s">
         <v>151</v>
       </c>
-      <c r="H42" s="78" t="s">
+      <c r="H45" s="78" t="s">
         <v>161</v>
       </c>
-      <c r="I42" s="78" t="s">
+      <c r="I45" s="78" t="s">
         <v>162</v>
       </c>
-      <c r="J42" s="90"/>
-    </row>
-    <row r="43" spans="2:10" ht="30" customHeight="1">
-      <c r="C43" s="52"/>
-      <c r="F43" s="6"/>
-      <c r="G43" s="7"/>
-      <c r="H43" s="11"/>
-    </row>
-    <row r="44" spans="2:10" ht="30">
-      <c r="B44" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="C44" s="49" t="s">
-        <v>119</v>
-      </c>
-      <c r="D44" s="20" t="s">
-        <v>120</v>
-      </c>
-      <c r="E44" s="21">
-        <v>42745</v>
-      </c>
-      <c r="F44" s="22" t="s">
-        <v>107</v>
-      </c>
-      <c r="G44" s="23" t="s">
-        <v>121</v>
-      </c>
-      <c r="H44" s="24" t="s">
-        <v>122</v>
-      </c>
-      <c r="I44" s="20" t="s">
-        <v>123</v>
-      </c>
-      <c r="J44" s="67"/>
-    </row>
-    <row r="45" spans="2:10" ht="75">
-      <c r="B45" s="72" t="s">
-        <v>16</v>
-      </c>
-      <c r="C45" s="73" t="s">
-        <v>119</v>
-      </c>
-      <c r="D45" s="87" t="s">
-        <v>188</v>
-      </c>
-      <c r="E45" s="75">
-        <v>42860</v>
-      </c>
-      <c r="F45" s="29" t="s">
-        <v>98</v>
-      </c>
-      <c r="G45" s="30" t="s">
-        <v>187</v>
-      </c>
-      <c r="H45" s="78" t="s">
-        <v>189</v>
-      </c>
-      <c r="I45" s="78" t="s">
-        <v>190</v>
-      </c>
-      <c r="J45" s="77"/>
+      <c r="J45" s="90"/>
     </row>
     <row r="46" spans="2:10" ht="30" customHeight="1">
       <c r="C46" s="52"/>
@@ -2472,207 +2547,267 @@
       <c r="G46" s="7"/>
       <c r="H46" s="11"/>
     </row>
-    <row r="47" spans="2:10" ht="45">
+    <row r="47" spans="2:10" ht="30">
       <c r="B47" s="19" t="s">
         <v>16</v>
       </c>
       <c r="C47" s="49" t="s">
-        <v>18</v>
+        <v>119</v>
       </c>
       <c r="D47" s="20" t="s">
-        <v>14</v>
+        <v>120</v>
       </c>
       <c r="E47" s="21">
-        <v>42734</v>
+        <v>42745</v>
       </c>
       <c r="F47" s="22" t="s">
         <v>107</v>
       </c>
-      <c r="G47" s="23"/>
+      <c r="G47" s="23" t="s">
+        <v>121</v>
+      </c>
       <c r="H47" s="24" t="s">
-        <v>25</v>
-      </c>
-      <c r="I47" s="20"/>
+        <v>122</v>
+      </c>
+      <c r="I47" s="20" t="s">
+        <v>123</v>
+      </c>
       <c r="J47" s="67"/>
     </row>
-    <row r="48" spans="2:10" ht="30" customHeight="1">
-      <c r="C48" s="52"/>
-      <c r="F48" s="6"/>
-      <c r="G48" s="7"/>
-      <c r="H48" s="11"/>
-    </row>
-    <row r="49" spans="2:10" ht="60">
-      <c r="B49" s="43" t="s">
-        <v>16</v>
-      </c>
-      <c r="C49" s="55" t="s">
-        <v>20</v>
-      </c>
-      <c r="D49" s="33"/>
-      <c r="E49" s="44">
-        <v>42709</v>
-      </c>
-      <c r="F49" s="45" t="s">
+    <row r="48" spans="2:10" ht="75">
+      <c r="B48" s="72" t="s">
+        <v>16</v>
+      </c>
+      <c r="C48" s="73" t="s">
+        <v>119</v>
+      </c>
+      <c r="D48" s="87" t="s">
+        <v>188</v>
+      </c>
+      <c r="E48" s="75">
+        <v>42860</v>
+      </c>
+      <c r="F48" s="29" t="s">
         <v>98</v>
       </c>
-      <c r="G49" s="46"/>
-      <c r="H49" s="47" t="s">
-        <v>21</v>
-      </c>
-      <c r="I49" s="47" t="s">
-        <v>24</v>
-      </c>
-      <c r="J49" s="70" t="s">
-        <v>139</v>
-      </c>
+      <c r="G48" s="30" t="s">
+        <v>187</v>
+      </c>
+      <c r="H48" s="78" t="s">
+        <v>189</v>
+      </c>
+      <c r="I48" s="78" t="s">
+        <v>190</v>
+      </c>
+      <c r="J48" s="77"/>
+    </row>
+    <row r="49" spans="2:10" ht="30" customHeight="1">
+      <c r="C49" s="52"/>
+      <c r="F49" s="6"/>
+      <c r="G49" s="7"/>
+      <c r="H49" s="11"/>
     </row>
     <row r="50" spans="2:10" ht="45">
       <c r="B50" s="19" t="s">
         <v>16</v>
       </c>
       <c r="C50" s="49" t="s">
-        <v>20</v>
-      </c>
-      <c r="D50" s="20"/>
+        <v>18</v>
+      </c>
+      <c r="D50" s="20" t="s">
+        <v>14</v>
+      </c>
       <c r="E50" s="21">
-        <v>42749</v>
+        <v>42734</v>
       </c>
       <c r="F50" s="22" t="s">
         <v>107</v>
       </c>
-      <c r="G50" s="20"/>
+      <c r="G50" s="23"/>
       <c r="H50" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="I50" s="20"/>
+      <c r="J50" s="67"/>
+    </row>
+    <row r="51" spans="2:10" ht="30" customHeight="1">
+      <c r="C51" s="52"/>
+      <c r="F51" s="6"/>
+      <c r="G51" s="7"/>
+      <c r="H51" s="11"/>
+    </row>
+    <row r="52" spans="2:10" ht="60">
+      <c r="B52" s="43" t="s">
+        <v>16</v>
+      </c>
+      <c r="C52" s="55" t="s">
+        <v>20</v>
+      </c>
+      <c r="D52" s="33"/>
+      <c r="E52" s="44">
+        <v>42709</v>
+      </c>
+      <c r="F52" s="45" t="s">
+        <v>98</v>
+      </c>
+      <c r="G52" s="46"/>
+      <c r="H52" s="47" t="s">
+        <v>21</v>
+      </c>
+      <c r="I52" s="47" t="s">
+        <v>24</v>
+      </c>
+      <c r="J52" s="70" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="53" spans="2:10" ht="45">
+      <c r="B53" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="C53" s="49" t="s">
+        <v>20</v>
+      </c>
+      <c r="D53" s="20"/>
+      <c r="E53" s="21">
+        <v>42749</v>
+      </c>
+      <c r="F53" s="22" t="s">
+        <v>107</v>
+      </c>
+      <c r="G53" s="20"/>
+      <c r="H53" s="24" t="s">
         <v>69</v>
       </c>
-      <c r="I50" s="24" t="s">
+      <c r="I53" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="J50" s="67"/>
-    </row>
-    <row r="51" spans="2:10" ht="30">
-      <c r="B51" s="34" t="s">
-        <v>16</v>
-      </c>
-      <c r="C51" s="50" t="s">
+      <c r="J53" s="67"/>
+    </row>
+    <row r="54" spans="2:10" ht="30">
+      <c r="B54" s="34" t="s">
+        <v>16</v>
+      </c>
+      <c r="C54" s="50" t="s">
         <v>20</v>
       </c>
-      <c r="D51" s="35"/>
-      <c r="E51" s="36">
+      <c r="D54" s="35"/>
+      <c r="E54" s="36">
         <v>42809</v>
       </c>
-      <c r="F51" s="37" t="s">
+      <c r="F54" s="37" t="s">
         <v>97</v>
       </c>
-      <c r="G51" s="40"/>
-      <c r="H51" s="38" t="s">
+      <c r="G54" s="40"/>
+      <c r="H54" s="38" t="s">
         <v>154</v>
       </c>
-      <c r="I51" s="38" t="s">
+      <c r="I54" s="38" t="s">
         <v>155</v>
       </c>
-      <c r="J51" s="66"/>
-    </row>
-    <row r="53" spans="2:10" ht="28.5" customHeight="1">
-      <c r="B53" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="C53" s="54" t="s">
+      <c r="J54" s="66"/>
+    </row>
+    <row r="56" spans="2:10" ht="28.5" customHeight="1">
+      <c r="B56" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C56" s="54" t="s">
         <v>176</v>
       </c>
-      <c r="D53" s="14" t="s">
+      <c r="D56" s="14" t="s">
         <v>133</v>
       </c>
-      <c r="E53" s="18">
+      <c r="E56" s="18">
         <v>42781</v>
       </c>
-      <c r="F53" s="13" t="s">
+      <c r="F56" s="13" t="s">
         <v>136</v>
       </c>
-      <c r="G53" s="14" t="s">
+      <c r="G56" s="14" t="s">
         <v>134</v>
       </c>
-      <c r="H53" s="15" t="s">
+      <c r="H56" s="15" t="s">
         <v>135</v>
       </c>
-      <c r="I53" s="14"/>
-      <c r="J53" s="69"/>
-    </row>
-    <row r="54" spans="2:10" ht="30">
-      <c r="B54" s="43" t="s">
-        <v>16</v>
-      </c>
-      <c r="C54" s="55" t="s">
+      <c r="I56" s="14"/>
+      <c r="J56" s="69"/>
+    </row>
+    <row r="57" spans="2:10" ht="30">
+      <c r="B57" s="43" t="s">
+        <v>16</v>
+      </c>
+      <c r="C57" s="55" t="s">
         <v>176</v>
       </c>
-      <c r="D54" s="33" t="s">
+      <c r="D57" s="33" t="s">
         <v>177</v>
       </c>
-      <c r="E54" s="44">
+      <c r="E57" s="44">
         <v>42468</v>
       </c>
-      <c r="F54" s="45" t="s">
+      <c r="F57" s="45" t="s">
         <v>136</v>
       </c>
-      <c r="G54" s="46" t="s">
+      <c r="G57" s="46" t="s">
         <v>186</v>
       </c>
-      <c r="H54" s="47" t="s">
+      <c r="H57" s="47" t="s">
         <v>178</v>
       </c>
-      <c r="I54" s="47"/>
-      <c r="J54" s="70"/>
-    </row>
-    <row r="55" spans="2:10" ht="30">
-      <c r="B55" s="43" t="s">
-        <v>16</v>
-      </c>
-      <c r="C55" s="55" t="s">
+      <c r="I57" s="47"/>
+      <c r="J57" s="70"/>
+    </row>
+    <row r="58" spans="2:10" ht="30">
+      <c r="B58" s="43" t="s">
+        <v>16</v>
+      </c>
+      <c r="C58" s="55" t="s">
         <v>176</v>
       </c>
-      <c r="D55" s="33" t="s">
+      <c r="D58" s="33" t="s">
         <v>179</v>
       </c>
-      <c r="E55" s="44">
+      <c r="E58" s="44">
         <v>42451</v>
       </c>
-      <c r="F55" s="45" t="s">
+      <c r="F58" s="45" t="s">
         <v>136</v>
       </c>
-      <c r="G55" s="46" t="s">
+      <c r="G58" s="46" t="s">
         <v>185</v>
       </c>
-      <c r="H55" s="47" t="s">
+      <c r="H58" s="47" t="s">
         <v>180</v>
       </c>
-      <c r="I55" s="47"/>
-      <c r="J55" s="70"/>
-    </row>
-    <row r="56" spans="2:10" ht="45">
-      <c r="B56" s="43" t="s">
-        <v>16</v>
-      </c>
-      <c r="C56" s="55" t="s">
+      <c r="I58" s="47"/>
+      <c r="J58" s="70"/>
+    </row>
+    <row r="59" spans="2:10" ht="45">
+      <c r="B59" s="43" t="s">
+        <v>16</v>
+      </c>
+      <c r="C59" s="55" t="s">
         <v>176</v>
       </c>
-      <c r="D56" s="33" t="s">
+      <c r="D59" s="33" t="s">
         <v>181</v>
       </c>
-      <c r="E56" s="44">
+      <c r="E59" s="44">
         <v>42488</v>
       </c>
-      <c r="F56" s="45" t="s">
+      <c r="F59" s="45" t="s">
         <v>136</v>
       </c>
-      <c r="G56" s="46" t="s">
+      <c r="G59" s="46" t="s">
         <v>184</v>
       </c>
-      <c r="H56" s="47" t="s">
+      <c r="H59" s="47" t="s">
         <v>182</v>
       </c>
-      <c r="I56" s="47" t="s">
+      <c r="I59" s="47" t="s">
         <v>183</v>
       </c>
-      <c r="J56" s="70"/>
+      <c r="J59" s="70"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2685,10 +2820,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:M32"/>
+  <dimension ref="B2:M33"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2707,17 +2842,17 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:13" ht="21">
-      <c r="B2" s="102" t="s">
+      <c r="B2" s="107" t="s">
         <v>138</v>
       </c>
-      <c r="C2" s="102"/>
-      <c r="D2" s="102"/>
-      <c r="E2" s="102"/>
-      <c r="F2" s="102"/>
-      <c r="G2" s="102"/>
-      <c r="H2" s="102"/>
-      <c r="I2" s="102"/>
-      <c r="J2" s="102"/>
+      <c r="C2" s="107"/>
+      <c r="D2" s="107"/>
+      <c r="E2" s="107"/>
+      <c r="F2" s="107"/>
+      <c r="G2" s="107"/>
+      <c r="H2" s="107"/>
+      <c r="I2" s="107"/>
+      <c r="J2" s="107"/>
     </row>
     <row r="4" spans="2:13" s="8" customFormat="1">
       <c r="B4" s="3" t="s">
@@ -3266,33 +3401,35 @@
       <c r="I28" s="92"/>
       <c r="J28" s="92"/>
     </row>
-    <row r="29" spans="2:10" ht="30" customHeight="1"/>
-    <row r="30" spans="2:10" ht="45">
-      <c r="B30" s="26" t="s">
+    <row r="29" spans="2:10" ht="60">
+      <c r="B29" s="103" t="s">
         <v>37</v>
       </c>
-      <c r="C30" s="51" t="s">
-        <v>81</v>
-      </c>
-      <c r="D30" s="27" t="s">
-        <v>85</v>
-      </c>
-      <c r="E30" s="28">
-        <v>42750</v>
-      </c>
-      <c r="F30" s="29" t="s">
-        <v>98</v>
-      </c>
-      <c r="G30" s="27" t="s">
-        <v>83</v>
-      </c>
-      <c r="H30" s="31" t="s">
-        <v>84</v>
-      </c>
-      <c r="I30" s="31"/>
-      <c r="J30" s="32"/>
-    </row>
-    <row r="31" spans="2:10" ht="60">
+      <c r="C29" s="49" t="s">
+        <v>166</v>
+      </c>
+      <c r="D29" s="101" t="s">
+        <v>224</v>
+      </c>
+      <c r="E29" s="21">
+        <v>42996</v>
+      </c>
+      <c r="F29" s="93" t="s">
+        <v>107</v>
+      </c>
+      <c r="G29" s="106" t="s">
+        <v>218</v>
+      </c>
+      <c r="H29" s="71" t="s">
+        <v>225</v>
+      </c>
+      <c r="I29" s="71" t="s">
+        <v>226</v>
+      </c>
+      <c r="J29" s="67"/>
+    </row>
+    <row r="30" spans="2:10" ht="30" customHeight="1"/>
+    <row r="31" spans="2:10" ht="45">
       <c r="B31" s="26" t="s">
         <v>37</v>
       </c>
@@ -3308,18 +3445,16 @@
       <c r="F31" s="29" t="s">
         <v>98</v>
       </c>
-      <c r="G31" s="30" t="s">
-        <v>82</v>
+      <c r="G31" s="27" t="s">
+        <v>83</v>
       </c>
       <c r="H31" s="31" t="s">
-        <v>79</v>
-      </c>
-      <c r="I31" s="31" t="s">
-        <v>80</v>
-      </c>
+        <v>84</v>
+      </c>
+      <c r="I31" s="31"/>
       <c r="J31" s="32"/>
     </row>
-    <row r="32" spans="2:10" ht="30">
+    <row r="32" spans="2:10" ht="60">
       <c r="B32" s="26" t="s">
         <v>37</v>
       </c>
@@ -3327,7 +3462,7 @@
         <v>81</v>
       </c>
       <c r="D32" s="27" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E32" s="28">
         <v>42750</v>
@@ -3336,15 +3471,42 @@
         <v>98</v>
       </c>
       <c r="G32" s="30" t="s">
+        <v>82</v>
+      </c>
+      <c r="H32" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="I32" s="31" t="s">
+        <v>80</v>
+      </c>
+      <c r="J32" s="32"/>
+    </row>
+    <row r="33" spans="2:10" ht="30">
+      <c r="B33" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="C33" s="51" t="s">
+        <v>81</v>
+      </c>
+      <c r="D33" s="27" t="s">
+        <v>86</v>
+      </c>
+      <c r="E33" s="28">
+        <v>42750</v>
+      </c>
+      <c r="F33" s="29" t="s">
+        <v>98</v>
+      </c>
+      <c r="G33" s="30" t="s">
         <v>87</v>
       </c>
-      <c r="H32" s="31" t="s">
+      <c r="H33" s="31" t="s">
         <v>88</v>
       </c>
-      <c r="I32" s="31" t="s">
+      <c r="I33" s="31" t="s">
         <v>89</v>
       </c>
-      <c r="J32" s="32"/>
+      <c r="J33" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
!U sync to live trunk from dev branch
</commit_message>
<xml_diff>
--- a/Codebase_Tracker.xlsx
+++ b/Codebase_Tracker.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="ProPack" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="283">
   <si>
     <t>Module</t>
   </si>
@@ -579,18 +579,9 @@
     <t>New Rig Manager</t>
   </si>
   <si>
-    <t>blends_target_missing_indexes_test</t>
-  </si>
-  <si>
     <t>New HealthTest</t>
   </si>
   <si>
-    <t>New test to check for blank/deleted targets on a BlendNode and force fix them</t>
-  </si>
-  <si>
-    <t>This is an issue with the FBX output of blendNodes. If you have a blendshape where you've deleted targets then that will cause issues in the fbx output as these empty indexes get removed from the node data but NOT the animation indexes. Causes issues in Unreal</t>
-  </si>
-  <si>
     <t>dynamic timecode added</t>
   </si>
   <si>
@@ -784,6 +775,96 @@
   </si>
   <si>
     <t xml:space="preserve">float3 handling in the addAttr was failing </t>
+  </si>
+  <si>
+    <t>isMetaNodeInherited</t>
+  </si>
+  <si>
+    <t>Re-written the whole subclass and registry management, added new global var that tracks each classes inheritance map but is able to have the keys looked up in short form rather than full issubclass call</t>
+  </si>
+  <si>
+    <t>This is to by-opass issue where a class may be instanitated several times during boot-up and from different setups. This was failing our internal developoment code as we have 2 branches and couldn't always check subclasses in the standard manner.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pro_MetaRig_FacialUI </t>
+  </si>
+  <si>
+    <t>BIG update to this base facial class to support custom modelPanel views, camera creation and alignment, imageplane management and a new head_instancer call to allow you to draw front, side_left and side_right in the viewports</t>
+  </si>
+  <si>
+    <t>This all relies on the mClass node being wired to the head meshes via the "renderMeshes" wire on the class</t>
+  </si>
+  <si>
+    <t>FilterNode</t>
+  </si>
+  <si>
+    <t>Possible to have duplicate nodes in the lists if nodeTypes included shape and transforms</t>
+  </si>
+  <si>
+    <t>Added extra catches to the lsSearchNodeTypes call</t>
+  </si>
+  <si>
+    <t>snapTransforms</t>
+  </si>
+  <si>
+    <t>AnimFunctions.snapTransform</t>
+  </si>
+  <si>
+    <t>New flag added additionalFuncs=[] which allows us to pass in a list of additional function calls to the process.</t>
+  </si>
+  <si>
+    <t>This allows us to add new functionality whilst only parsing time once, and managing the threading etc</t>
+  </si>
+  <si>
+    <t>r9General</t>
+  </si>
+  <si>
+    <t>decorator</t>
+  </si>
+  <si>
+    <t>deleteNewNodes</t>
+  </si>
+  <si>
+    <t>New decorator that deletes any nodes generated by the function being decorated</t>
+  </si>
+  <si>
+    <t>P4_sourceControl</t>
+  </si>
+  <si>
+    <t>ALL Properties converted back to function calls</t>
+  </si>
+  <si>
+    <t>With some of the Perforce calls being properties it was massively slowing down code completion in Maya, all properties in the current P4 bindings have been removed, things like .fstat will now need to be called as functions .fstat()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New Project call "p4_switch_streams" which now allows you to dynamically change the current P4 stream/client mount. </t>
+  </si>
+  <si>
+    <t>Really useful if you have P4 setup with multiple mounts/clients in the same workspace</t>
+  </si>
+  <si>
+    <t>fk_ik_match and methods for resolving the ik and fk chains have been uplifted</t>
+  </si>
+  <si>
+    <t>ikimatchpnt now has a pointer to the controller it relates too, these used to be hard-coded. New method for matching the toe data added which relies on a new patch.</t>
+  </si>
+  <si>
+    <t>When dealing with mRigs theres now a new popupmenu thats triggered when you rmb click over the "MetaRoot" button. This presents a menu with all found mRigs in the scene to choose from. It also exposes a new "Auto-Resolved" option that will bind all operations to the rig found from the currently selected.</t>
+  </si>
+  <si>
+    <t>This is a workflow speedup, saving animators from having to continually set the MetaRoot in the UI. Instead the pose will load onto the rig found from the selected controller.</t>
+  </si>
+  <si>
+    <t>r9ie.P4_sourceControl</t>
+  </si>
+  <si>
+    <t>Massive update to the P4 handling and how we're wrapping it. All previous property's have been turned back to functions for speed in the Maya scriptEditor. Lots of additional logic in the hadnling added for better debuging and stability in the connection.</t>
+  </si>
+  <si>
+    <t>This is TOTALLY dependent on the PROJECT_DATA object's P4 bindings</t>
+  </si>
+  <si>
+    <t>!!</t>
   </si>
 </sst>
 </file>
@@ -793,7 +874,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -863,6 +944,14 @@
     <font>
       <b/>
       <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="28"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -971,7 +1060,7 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="109">
+  <cellXfs count="118">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1294,8 +1383,35 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="4" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="4" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="5" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="5" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="4" borderId="3" xfId="5" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="5" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="5" borderId="2" xfId="4" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="4" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="4" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -1610,10 +1726,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:M64"/>
+  <dimension ref="A2:M69"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="F64" sqref="F64"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="D58" sqref="D58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1632,17 +1748,17 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:13" ht="21">
-      <c r="B2" s="108" t="s">
+      <c r="B2" s="116" t="s">
         <v>137</v>
       </c>
-      <c r="C2" s="108"/>
-      <c r="D2" s="108"/>
-      <c r="E2" s="108"/>
-      <c r="F2" s="108"/>
-      <c r="G2" s="108"/>
-      <c r="H2" s="108"/>
-      <c r="I2" s="108"/>
-      <c r="J2" s="108"/>
+      <c r="C2" s="116"/>
+      <c r="D2" s="116"/>
+      <c r="E2" s="116"/>
+      <c r="F2" s="116"/>
+      <c r="G2" s="116"/>
+      <c r="H2" s="116"/>
+      <c r="I2" s="116"/>
+      <c r="J2" s="116"/>
     </row>
     <row r="3" spans="1:13" ht="15.6" customHeight="1"/>
     <row r="4" spans="1:13" s="2" customFormat="1" ht="24" customHeight="1">
@@ -1840,7 +1956,7 @@
         <v>107</v>
       </c>
       <c r="M12" s="98" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="45">
@@ -1893,7 +2009,7 @@
         <v>107</v>
       </c>
       <c r="G14" s="91" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H14" s="71" t="s">
         <v>168</v>
@@ -1920,13 +2036,13 @@
         <v>98</v>
       </c>
       <c r="G15" s="30" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="H15" s="78" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="I15" s="78" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="J15" s="77"/>
     </row>
@@ -1938,7 +2054,7 @@
         <v>28</v>
       </c>
       <c r="D16" s="87" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="E16" s="75">
         <v>42983</v>
@@ -1947,13 +2063,13 @@
         <v>98</v>
       </c>
       <c r="G16" s="102" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="H16" s="78" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="I16" s="78" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="J16" s="77"/>
     </row>
@@ -1974,13 +2090,13 @@
         <v>107</v>
       </c>
       <c r="G17" s="106" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="H17" s="71" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="I17" s="71" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="J17" s="67"/>
     </row>
@@ -2001,13 +2117,13 @@
         <v>98</v>
       </c>
       <c r="G18" s="102" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="H18" s="78" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="I18" s="78" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="J18" s="77"/>
     </row>
@@ -2019,7 +2135,7 @@
         <v>28</v>
       </c>
       <c r="D19" s="87" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="E19" s="75">
         <v>43023</v>
@@ -2028,13 +2144,13 @@
         <v>98</v>
       </c>
       <c r="G19" s="102" t="s">
+        <v>229</v>
+      </c>
+      <c r="H19" s="78" t="s">
+        <v>231</v>
+      </c>
+      <c r="I19" s="78" t="s">
         <v>232</v>
-      </c>
-      <c r="H19" s="78" t="s">
-        <v>234</v>
-      </c>
-      <c r="I19" s="78" t="s">
-        <v>235</v>
       </c>
       <c r="J19" s="77"/>
     </row>
@@ -2055,13 +2171,13 @@
         <v>107</v>
       </c>
       <c r="G20" s="106" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="H20" s="71" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="I20" s="71" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="J20" s="67"/>
     </row>
@@ -2138,13 +2254,13 @@
         <v>98</v>
       </c>
       <c r="G24" s="30" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="H24" s="31" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="I24" s="31" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="J24" s="68"/>
     </row>
@@ -2536,13 +2652,13 @@
         <v>107</v>
       </c>
       <c r="G41" s="91" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="H41" s="71" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="I41" s="71" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="J41" s="105"/>
     </row>
@@ -2563,75 +2679,77 @@
         <v>98</v>
       </c>
       <c r="G42" s="30" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="H42" s="31" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="I42" s="31" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="J42" s="68"/>
     </row>
-    <row r="43" spans="2:10" ht="30" customHeight="1">
-      <c r="C43" s="52"/>
-      <c r="F43" s="6"/>
-      <c r="G43" s="7"/>
-      <c r="H43" s="11"/>
-    </row>
-    <row r="44" spans="2:10" ht="60">
-      <c r="B44" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="C44" s="49" t="s">
-        <v>13</v>
-      </c>
-      <c r="D44" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="E44" s="21">
-        <v>42734</v>
-      </c>
-      <c r="F44" s="22" t="s">
-        <v>107</v>
-      </c>
-      <c r="G44" s="23" t="s">
-        <v>53</v>
-      </c>
-      <c r="H44" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="I44" s="24" t="s">
-        <v>132</v>
-      </c>
-      <c r="J44" s="67"/>
-    </row>
-    <row r="45" spans="2:10" ht="45">
-      <c r="B45" s="34" t="s">
-        <v>16</v>
-      </c>
-      <c r="C45" s="50" t="s">
-        <v>13</v>
-      </c>
-      <c r="D45" s="35" t="s">
-        <v>13</v>
-      </c>
-      <c r="E45" s="36">
-        <v>42740</v>
-      </c>
-      <c r="F45" s="37" t="s">
+    <row r="43" spans="2:10" ht="60">
+      <c r="B43" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="C43" s="51" t="s">
+        <v>17</v>
+      </c>
+      <c r="D43" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="E43" s="28">
+        <v>43080</v>
+      </c>
+      <c r="F43" s="29" t="s">
+        <v>98</v>
+      </c>
+      <c r="G43" s="30" t="s">
+        <v>256</v>
+      </c>
+      <c r="H43" s="31" t="s">
+        <v>257</v>
+      </c>
+      <c r="I43" s="31" t="s">
+        <v>258</v>
+      </c>
+      <c r="J43" s="68"/>
+    </row>
+    <row r="44" spans="2:10" ht="45">
+      <c r="B44" s="109" t="s">
+        <v>16</v>
+      </c>
+      <c r="C44" s="110" t="s">
+        <v>17</v>
+      </c>
+      <c r="D44" s="110" t="s">
+        <v>41</v>
+      </c>
+      <c r="E44" s="59">
+        <v>43110</v>
+      </c>
+      <c r="F44" s="111" t="s">
         <v>97</v>
       </c>
-      <c r="G45" s="40" t="s">
-        <v>75</v>
-      </c>
-      <c r="H45" s="38" t="s">
-        <v>44</v>
-      </c>
-      <c r="I45" s="35"/>
-      <c r="J45" s="66"/>
-    </row>
-    <row r="46" spans="2:10" ht="45">
+      <c r="G44" s="40" t="s">
+        <v>41</v>
+      </c>
+      <c r="H44" s="38" t="s">
+        <v>275</v>
+      </c>
+      <c r="I44" s="38" t="s">
+        <v>276</v>
+      </c>
+      <c r="J44" s="112"/>
+    </row>
+    <row r="45" spans="2:10" ht="30" customHeight="1">
+      <c r="C45" s="52"/>
+      <c r="F45" s="6"/>
+      <c r="G45" s="7"/>
+      <c r="H45" s="11"/>
+    </row>
+    <row r="46" spans="2:10" ht="60">
       <c r="B46" s="19" t="s">
         <v>16</v>
       </c>
@@ -2642,397 +2760,529 @@
         <v>13</v>
       </c>
       <c r="E46" s="21">
-        <v>42745</v>
+        <v>42734</v>
       </c>
       <c r="F46" s="22" t="s">
         <v>107</v>
       </c>
       <c r="G46" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="H46" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="I46" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="J46" s="67"/>
+    </row>
+    <row r="47" spans="2:10" ht="45">
+      <c r="B47" s="34" t="s">
+        <v>16</v>
+      </c>
+      <c r="C47" s="50" t="s">
+        <v>13</v>
+      </c>
+      <c r="D47" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="E47" s="36">
+        <v>42740</v>
+      </c>
+      <c r="F47" s="37" t="s">
+        <v>97</v>
+      </c>
+      <c r="G47" s="40" t="s">
+        <v>75</v>
+      </c>
+      <c r="H47" s="38" t="s">
+        <v>44</v>
+      </c>
+      <c r="I47" s="35"/>
+      <c r="J47" s="66"/>
+    </row>
+    <row r="48" spans="2:10" ht="45">
+      <c r="B48" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="C48" s="49" t="s">
+        <v>13</v>
+      </c>
+      <c r="D48" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="E48" s="21">
+        <v>42745</v>
+      </c>
+      <c r="F48" s="22" t="s">
+        <v>107</v>
+      </c>
+      <c r="G48" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="H46" s="24" t="s">
+      <c r="H48" s="24" t="s">
         <v>64</v>
       </c>
-      <c r="I46" s="20" t="s">
+      <c r="I48" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="J46" s="67"/>
-    </row>
-    <row r="47" spans="2:10" ht="45">
-      <c r="B47" s="79" t="s">
-        <v>16</v>
-      </c>
-      <c r="C47" s="80" t="s">
+      <c r="J48" s="67"/>
+    </row>
+    <row r="49" spans="1:10" ht="45">
+      <c r="B49" s="79" t="s">
+        <v>16</v>
+      </c>
+      <c r="C49" s="80" t="s">
         <v>13</v>
       </c>
-      <c r="D47" s="83" t="s">
+      <c r="D49" s="83" t="s">
         <v>13</v>
       </c>
-      <c r="E47" s="81">
+      <c r="E49" s="81">
         <v>42811</v>
       </c>
-      <c r="F47" s="13" t="s">
+      <c r="F49" s="13" t="s">
         <v>136</v>
       </c>
-      <c r="G47" s="46" t="s">
+      <c r="G49" s="46" t="s">
         <v>151</v>
       </c>
-      <c r="H47" s="84" t="s">
+      <c r="H49" s="84" t="s">
         <v>152</v>
       </c>
-      <c r="I47" s="83" t="s">
+      <c r="I49" s="83" t="s">
         <v>153</v>
       </c>
-      <c r="J47" s="82"/>
-    </row>
-    <row r="48" spans="2:10" ht="45">
-      <c r="B48" s="86" t="s">
-        <v>16</v>
-      </c>
-      <c r="C48" s="73" t="s">
+      <c r="J49" s="82"/>
+    </row>
+    <row r="50" spans="1:10" ht="45">
+      <c r="B50" s="86" t="s">
+        <v>16</v>
+      </c>
+      <c r="C50" s="73" t="s">
         <v>13</v>
       </c>
-      <c r="D48" s="87" t="s">
+      <c r="D50" s="87" t="s">
         <v>13</v>
       </c>
-      <c r="E48" s="88">
+      <c r="E50" s="88">
         <v>42817</v>
       </c>
-      <c r="F48" s="89" t="s">
+      <c r="F50" s="89" t="s">
         <v>98</v>
       </c>
-      <c r="G48" s="30" t="s">
+      <c r="G50" s="30" t="s">
         <v>151</v>
       </c>
-      <c r="H48" s="78" t="s">
+      <c r="H50" s="78" t="s">
         <v>161</v>
       </c>
-      <c r="I48" s="78" t="s">
+      <c r="I50" s="78" t="s">
         <v>162</v>
       </c>
-      <c r="J48" s="90"/>
-    </row>
-    <row r="49" spans="2:10" ht="30" customHeight="1">
-      <c r="C49" s="52"/>
-      <c r="F49" s="6"/>
-      <c r="G49" s="7"/>
-      <c r="H49" s="11"/>
-    </row>
-    <row r="50" spans="2:10" ht="30">
-      <c r="B50" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="C50" s="49" t="s">
-        <v>119</v>
-      </c>
-      <c r="D50" s="20" t="s">
-        <v>120</v>
-      </c>
-      <c r="E50" s="21">
-        <v>42745</v>
-      </c>
-      <c r="F50" s="22" t="s">
-        <v>107</v>
-      </c>
-      <c r="G50" s="23" t="s">
-        <v>121</v>
-      </c>
-      <c r="H50" s="24" t="s">
-        <v>122</v>
-      </c>
-      <c r="I50" s="20" t="s">
-        <v>123</v>
-      </c>
-      <c r="J50" s="67"/>
-    </row>
-    <row r="51" spans="2:10" ht="75">
-      <c r="B51" s="72" t="s">
+      <c r="J50" s="90"/>
+    </row>
+    <row r="51" spans="1:10" ht="30">
+      <c r="B51" s="86" t="s">
         <v>16</v>
       </c>
       <c r="C51" s="73" t="s">
-        <v>119</v>
+        <v>13</v>
       </c>
       <c r="D51" s="87" t="s">
-        <v>188</v>
-      </c>
-      <c r="E51" s="75">
-        <v>42860</v>
-      </c>
-      <c r="F51" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="E51" s="88">
+        <v>43110</v>
+      </c>
+      <c r="F51" s="89" t="s">
         <v>98</v>
       </c>
       <c r="G51" s="30" t="s">
-        <v>187</v>
+        <v>151</v>
       </c>
       <c r="H51" s="78" t="s">
-        <v>189</v>
+        <v>273</v>
       </c>
       <c r="I51" s="78" t="s">
-        <v>190</v>
-      </c>
-      <c r="J51" s="77"/>
-    </row>
-    <row r="52" spans="2:10" ht="30" customHeight="1">
+        <v>274</v>
+      </c>
+      <c r="J51" s="90"/>
+    </row>
+    <row r="52" spans="1:10" ht="30" customHeight="1">
       <c r="C52" s="52"/>
       <c r="F52" s="6"/>
       <c r="G52" s="7"/>
       <c r="H52" s="11"/>
     </row>
-    <row r="53" spans="2:10" ht="45">
+    <row r="53" spans="1:10" ht="30">
       <c r="B53" s="19" t="s">
         <v>16</v>
       </c>
       <c r="C53" s="49" t="s">
-        <v>18</v>
+        <v>119</v>
       </c>
       <c r="D53" s="20" t="s">
-        <v>14</v>
+        <v>120</v>
       </c>
       <c r="E53" s="21">
-        <v>42734</v>
+        <v>42745</v>
       </c>
       <c r="F53" s="22" t="s">
         <v>107</v>
       </c>
-      <c r="G53" s="23"/>
+      <c r="G53" s="23" t="s">
+        <v>121</v>
+      </c>
       <c r="H53" s="24" t="s">
-        <v>25</v>
-      </c>
-      <c r="I53" s="20"/>
+        <v>122</v>
+      </c>
+      <c r="I53" s="20" t="s">
+        <v>123</v>
+      </c>
       <c r="J53" s="67"/>
     </row>
-    <row r="54" spans="2:10" ht="30" customHeight="1">
-      <c r="C54" s="52"/>
-      <c r="F54" s="6"/>
-      <c r="G54" s="7"/>
-      <c r="H54" s="11"/>
-    </row>
-    <row r="55" spans="2:10" ht="60">
-      <c r="B55" s="43" t="s">
-        <v>16</v>
-      </c>
-      <c r="C55" s="55" t="s">
-        <v>20</v>
-      </c>
-      <c r="D55" s="33"/>
-      <c r="E55" s="44">
-        <v>42709</v>
-      </c>
-      <c r="F55" s="45" t="s">
-        <v>98</v>
-      </c>
-      <c r="G55" s="46"/>
-      <c r="H55" s="47" t="s">
-        <v>21</v>
-      </c>
-      <c r="I55" s="47" t="s">
-        <v>24</v>
-      </c>
-      <c r="J55" s="70" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="56" spans="2:10" ht="45">
+    <row r="54" spans="1:10" ht="60">
+      <c r="B54" s="72" t="s">
+        <v>16</v>
+      </c>
+      <c r="C54" s="73" t="s">
+        <v>119</v>
+      </c>
+      <c r="D54" s="87" t="s">
+        <v>187</v>
+      </c>
+      <c r="E54" s="75">
+        <v>43110</v>
+      </c>
+      <c r="F54" s="29" t="s">
+        <v>97</v>
+      </c>
+      <c r="G54" s="30" t="s">
+        <v>270</v>
+      </c>
+      <c r="H54" s="78" t="s">
+        <v>271</v>
+      </c>
+      <c r="I54" s="78" t="s">
+        <v>272</v>
+      </c>
+      <c r="J54" s="77"/>
+    </row>
+    <row r="55" spans="1:10" ht="30" customHeight="1">
+      <c r="C55" s="52"/>
+      <c r="F55" s="6"/>
+      <c r="G55" s="7"/>
+      <c r="H55" s="11"/>
+    </row>
+    <row r="56" spans="1:10" ht="45">
       <c r="B56" s="19" t="s">
         <v>16</v>
       </c>
       <c r="C56" s="49" t="s">
-        <v>20</v>
-      </c>
-      <c r="D56" s="20"/>
+        <v>18</v>
+      </c>
+      <c r="D56" s="20" t="s">
+        <v>14</v>
+      </c>
       <c r="E56" s="21">
-        <v>42749</v>
+        <v>42734</v>
       </c>
       <c r="F56" s="22" t="s">
         <v>107</v>
       </c>
-      <c r="G56" s="20"/>
+      <c r="G56" s="23"/>
       <c r="H56" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="I56" s="20"/>
+      <c r="J56" s="67"/>
+    </row>
+    <row r="57" spans="1:10" ht="45">
+      <c r="B57" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="C57" s="49" t="s">
+        <v>18</v>
+      </c>
+      <c r="D57" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="E57" s="21">
+        <v>42734</v>
+      </c>
+      <c r="F57" s="93" t="s">
+        <v>107</v>
+      </c>
+      <c r="G57" s="23"/>
+      <c r="H57" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="I57" s="20"/>
+      <c r="J57" s="67"/>
+    </row>
+    <row r="58" spans="1:10" ht="75">
+      <c r="A58" s="115" t="s">
+        <v>282</v>
+      </c>
+      <c r="B58" s="72" t="s">
+        <v>16</v>
+      </c>
+      <c r="C58" s="117" t="s">
+        <v>18</v>
+      </c>
+      <c r="D58" s="74" t="s">
+        <v>14</v>
+      </c>
+      <c r="E58" s="75">
+        <v>43110</v>
+      </c>
+      <c r="F58" s="113" t="s">
+        <v>97</v>
+      </c>
+      <c r="G58" s="76" t="s">
+        <v>279</v>
+      </c>
+      <c r="H58" s="114" t="s">
+        <v>280</v>
+      </c>
+      <c r="I58" s="74" t="s">
+        <v>281</v>
+      </c>
+      <c r="J58" s="77"/>
+    </row>
+    <row r="59" spans="1:10" ht="30" customHeight="1">
+      <c r="C59" s="52"/>
+      <c r="F59" s="6"/>
+      <c r="G59" s="7"/>
+      <c r="H59" s="11"/>
+    </row>
+    <row r="60" spans="1:10" ht="60">
+      <c r="B60" s="43" t="s">
+        <v>16</v>
+      </c>
+      <c r="C60" s="55" t="s">
+        <v>20</v>
+      </c>
+      <c r="D60" s="33"/>
+      <c r="E60" s="44">
+        <v>42709</v>
+      </c>
+      <c r="F60" s="45" t="s">
+        <v>98</v>
+      </c>
+      <c r="G60" s="46"/>
+      <c r="H60" s="47" t="s">
+        <v>21</v>
+      </c>
+      <c r="I60" s="47" t="s">
+        <v>24</v>
+      </c>
+      <c r="J60" s="70" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" ht="45">
+      <c r="B61" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="C61" s="49" t="s">
+        <v>20</v>
+      </c>
+      <c r="D61" s="20"/>
+      <c r="E61" s="21">
+        <v>42749</v>
+      </c>
+      <c r="F61" s="22" t="s">
+        <v>107</v>
+      </c>
+      <c r="G61" s="20"/>
+      <c r="H61" s="24" t="s">
         <v>69</v>
       </c>
-      <c r="I56" s="24" t="s">
+      <c r="I61" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="J56" s="67"/>
-    </row>
-    <row r="57" spans="2:10" ht="30">
-      <c r="B57" s="34" t="s">
-        <v>16</v>
-      </c>
-      <c r="C57" s="50" t="s">
+      <c r="J61" s="67"/>
+    </row>
+    <row r="62" spans="1:10" ht="30">
+      <c r="B62" s="34" t="s">
+        <v>16</v>
+      </c>
+      <c r="C62" s="50" t="s">
         <v>20</v>
       </c>
-      <c r="D57" s="35"/>
-      <c r="E57" s="36">
+      <c r="D62" s="35"/>
+      <c r="E62" s="36">
         <v>42809</v>
       </c>
-      <c r="F57" s="37" t="s">
+      <c r="F62" s="37" t="s">
         <v>97</v>
       </c>
-      <c r="G57" s="40"/>
-      <c r="H57" s="38" t="s">
+      <c r="G62" s="40"/>
+      <c r="H62" s="38" t="s">
         <v>154</v>
       </c>
-      <c r="I57" s="38" t="s">
+      <c r="I62" s="38" t="s">
         <v>155</v>
       </c>
-      <c r="J57" s="66"/>
-    </row>
-    <row r="59" spans="2:10" ht="28.5" customHeight="1">
-      <c r="B59" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="C59" s="54" t="s">
+      <c r="J62" s="66"/>
+    </row>
+    <row r="64" spans="1:10" ht="28.5" customHeight="1">
+      <c r="B64" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C64" s="54" t="s">
         <v>176</v>
       </c>
-      <c r="D59" s="14" t="s">
+      <c r="D64" s="14" t="s">
         <v>133</v>
       </c>
-      <c r="E59" s="18">
+      <c r="E64" s="18">
         <v>42781</v>
       </c>
-      <c r="F59" s="13" t="s">
+      <c r="F64" s="13" t="s">
         <v>136</v>
       </c>
-      <c r="G59" s="14" t="s">
+      <c r="G64" s="14" t="s">
         <v>134</v>
       </c>
-      <c r="H59" s="15" t="s">
+      <c r="H64" s="15" t="s">
         <v>135</v>
       </c>
-      <c r="I59" s="14"/>
-      <c r="J59" s="69"/>
-    </row>
-    <row r="60" spans="2:10" ht="30">
-      <c r="B60" s="43" t="s">
-        <v>16</v>
-      </c>
-      <c r="C60" s="55" t="s">
+      <c r="I64" s="14"/>
+      <c r="J64" s="69"/>
+    </row>
+    <row r="65" spans="2:10" ht="30">
+      <c r="B65" s="43" t="s">
+        <v>16</v>
+      </c>
+      <c r="C65" s="55" t="s">
         <v>176</v>
       </c>
-      <c r="D60" s="33" t="s">
+      <c r="D65" s="33" t="s">
         <v>177</v>
       </c>
-      <c r="E60" s="44">
+      <c r="E65" s="44">
         <v>42468</v>
       </c>
-      <c r="F60" s="45" t="s">
+      <c r="F65" s="45" t="s">
         <v>136</v>
       </c>
-      <c r="G60" s="46" t="s">
+      <c r="G65" s="46" t="s">
         <v>186</v>
       </c>
-      <c r="H60" s="47" t="s">
+      <c r="H65" s="47" t="s">
         <v>178</v>
       </c>
-      <c r="I60" s="47"/>
-      <c r="J60" s="70"/>
-    </row>
-    <row r="61" spans="2:10" ht="30">
-      <c r="B61" s="43" t="s">
-        <v>16</v>
-      </c>
-      <c r="C61" s="55" t="s">
+      <c r="I65" s="47"/>
+      <c r="J65" s="70"/>
+    </row>
+    <row r="66" spans="2:10" ht="30">
+      <c r="B66" s="43" t="s">
+        <v>16</v>
+      </c>
+      <c r="C66" s="55" t="s">
         <v>176</v>
       </c>
-      <c r="D61" s="33" t="s">
+      <c r="D66" s="33" t="s">
         <v>179</v>
       </c>
-      <c r="E61" s="44">
+      <c r="E66" s="44">
         <v>42451</v>
       </c>
-      <c r="F61" s="45" t="s">
+      <c r="F66" s="45" t="s">
         <v>136</v>
       </c>
-      <c r="G61" s="46" t="s">
+      <c r="G66" s="46" t="s">
         <v>185</v>
       </c>
-      <c r="H61" s="47" t="s">
+      <c r="H66" s="47" t="s">
         <v>180</v>
       </c>
-      <c r="I61" s="47"/>
-      <c r="J61" s="70"/>
-    </row>
-    <row r="62" spans="2:10" ht="45">
-      <c r="B62" s="43" t="s">
-        <v>16</v>
-      </c>
-      <c r="C62" s="55" t="s">
+      <c r="I66" s="47"/>
+      <c r="J66" s="70"/>
+    </row>
+    <row r="67" spans="2:10" ht="45">
+      <c r="B67" s="43" t="s">
+        <v>16</v>
+      </c>
+      <c r="C67" s="55" t="s">
         <v>176</v>
       </c>
-      <c r="D62" s="33" t="s">
+      <c r="D67" s="33" t="s">
         <v>181</v>
       </c>
-      <c r="E62" s="44">
+      <c r="E67" s="44">
         <v>42488</v>
       </c>
-      <c r="F62" s="45" t="s">
+      <c r="F67" s="45" t="s">
         <v>136</v>
       </c>
-      <c r="G62" s="46" t="s">
+      <c r="G67" s="46" t="s">
         <v>184</v>
       </c>
-      <c r="H62" s="47" t="s">
+      <c r="H67" s="47" t="s">
         <v>182</v>
       </c>
-      <c r="I62" s="47" t="s">
+      <c r="I67" s="47" t="s">
         <v>183</v>
       </c>
-      <c r="J62" s="70"/>
-    </row>
-    <row r="63" spans="2:10" ht="30">
-      <c r="B63" s="26" t="s">
-        <v>16</v>
-      </c>
-      <c r="C63" s="51" t="s">
+      <c r="J67" s="70"/>
+    </row>
+    <row r="68" spans="2:10" ht="30">
+      <c r="B68" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="C68" s="51" t="s">
         <v>176</v>
       </c>
-      <c r="D63" s="27" t="s">
+      <c r="D68" s="27" t="s">
         <v>181</v>
       </c>
-      <c r="E63" s="28">
+      <c r="E68" s="28">
         <v>43013</v>
       </c>
-      <c r="F63" s="29" t="s">
+      <c r="F68" s="29" t="s">
         <v>98</v>
       </c>
-      <c r="G63" s="30" t="s">
+      <c r="G68" s="30" t="s">
+        <v>246</v>
+      </c>
+      <c r="H68" s="31" t="s">
+        <v>224</v>
+      </c>
+      <c r="I68" s="31" t="s">
+        <v>225</v>
+      </c>
+      <c r="J68" s="68"/>
+    </row>
+    <row r="69" spans="2:10" ht="30">
+      <c r="B69" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="C69" s="51" t="s">
+        <v>176</v>
+      </c>
+      <c r="D69" s="27" t="s">
+        <v>181</v>
+      </c>
+      <c r="E69" s="28">
+        <v>43047</v>
+      </c>
+      <c r="F69" s="29" t="s">
+        <v>98</v>
+      </c>
+      <c r="G69" s="30" t="s">
+        <v>247</v>
+      </c>
+      <c r="H69" s="31" t="s">
+        <v>248</v>
+      </c>
+      <c r="I69" s="31" t="s">
         <v>249</v>
       </c>
-      <c r="H63" s="31" t="s">
-        <v>227</v>
-      </c>
-      <c r="I63" s="31" t="s">
-        <v>228</v>
-      </c>
-      <c r="J63" s="68"/>
-    </row>
-    <row r="64" spans="2:10" ht="30">
-      <c r="B64" s="26" t="s">
-        <v>16</v>
-      </c>
-      <c r="C64" s="51" t="s">
-        <v>176</v>
-      </c>
-      <c r="D64" s="27" t="s">
-        <v>181</v>
-      </c>
-      <c r="E64" s="28">
-        <v>43047</v>
-      </c>
-      <c r="F64" s="29" t="s">
-        <v>98</v>
-      </c>
-      <c r="G64" s="30" t="s">
-        <v>250</v>
-      </c>
-      <c r="H64" s="31" t="s">
-        <v>251</v>
-      </c>
-      <c r="I64" s="31" t="s">
-        <v>252</v>
-      </c>
-      <c r="J64" s="68"/>
+      <c r="J69" s="68"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3045,10 +3295,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:M37"/>
+  <dimension ref="B2:M43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3067,17 +3317,17 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:13" ht="21">
-      <c r="B2" s="108" t="s">
+      <c r="B2" s="116" t="s">
         <v>138</v>
       </c>
-      <c r="C2" s="108"/>
-      <c r="D2" s="108"/>
-      <c r="E2" s="108"/>
-      <c r="F2" s="108"/>
-      <c r="G2" s="108"/>
-      <c r="H2" s="108"/>
-      <c r="I2" s="108"/>
-      <c r="J2" s="108"/>
+      <c r="C2" s="116"/>
+      <c r="D2" s="116"/>
+      <c r="E2" s="116"/>
+      <c r="F2" s="116"/>
+      <c r="G2" s="116"/>
+      <c r="H2" s="116"/>
+      <c r="I2" s="116"/>
+      <c r="J2" s="116"/>
     </row>
     <row r="4" spans="2:13" s="8" customFormat="1">
       <c r="B4" s="3" t="s">
@@ -3145,7 +3395,7 @@
         <v>107</v>
       </c>
       <c r="M6" s="98" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
     </row>
     <row r="7" spans="2:13" ht="45">
@@ -3253,7 +3503,7 @@
         <v>101</v>
       </c>
       <c r="I11" s="31" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="J11" s="32"/>
     </row>
@@ -3301,13 +3551,13 @@
         <v>97</v>
       </c>
       <c r="G13" s="30" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="H13" s="31" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="I13" s="31" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="J13" s="32"/>
     </row>
@@ -3319,7 +3569,7 @@
         <v>5</v>
       </c>
       <c r="D14" s="35" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="E14" s="36">
         <v>42885</v>
@@ -3328,518 +3578,652 @@
         <v>97</v>
       </c>
       <c r="G14" s="40" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="H14" s="38" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="I14" s="38" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="J14" s="39"/>
     </row>
-    <row r="15" spans="2:13" ht="30" customHeight="1"/>
-    <row r="16" spans="2:13" ht="45">
-      <c r="B16" s="19" t="s">
+    <row r="15" spans="2:13" ht="30">
+      <c r="B15" s="34" t="s">
         <v>37</v>
       </c>
-      <c r="C16" s="49" t="s">
+      <c r="C15" s="50" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" s="35" t="s">
+        <v>262</v>
+      </c>
+      <c r="E15" s="36">
+        <v>43098</v>
+      </c>
+      <c r="F15" s="37" t="s">
+        <v>97</v>
+      </c>
+      <c r="G15" s="40" t="s">
+        <v>263</v>
+      </c>
+      <c r="H15" s="38" t="s">
+        <v>264</v>
+      </c>
+      <c r="I15" s="38" t="s">
+        <v>265</v>
+      </c>
+      <c r="J15" s="39"/>
+    </row>
+    <row r="16" spans="2:13" ht="90">
+      <c r="B16" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" s="51" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="E16" s="28">
+        <v>43128</v>
+      </c>
+      <c r="F16" s="29" t="s">
+        <v>98</v>
+      </c>
+      <c r="G16" s="30" t="s">
+        <v>198</v>
+      </c>
+      <c r="H16" s="31" t="s">
+        <v>277</v>
+      </c>
+      <c r="I16" s="31" t="s">
+        <v>278</v>
+      </c>
+      <c r="J16" s="32"/>
+    </row>
+    <row r="17" spans="2:10" ht="30" customHeight="1"/>
+    <row r="18" spans="2:10" ht="45">
+      <c r="B18" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" s="49" t="s">
         <v>102</v>
       </c>
-      <c r="D16" s="20" t="s">
+      <c r="D18" s="20" t="s">
         <v>103</v>
       </c>
-      <c r="E16" s="21">
+      <c r="E18" s="21">
         <v>42761</v>
       </c>
-      <c r="F16" s="22" t="s">
+      <c r="F18" s="22" t="s">
         <v>107</v>
       </c>
-      <c r="G16" s="23" t="s">
+      <c r="G18" s="23" t="s">
         <v>100</v>
       </c>
-      <c r="H16" s="24" t="s">
+      <c r="H18" s="24" t="s">
         <v>104</v>
       </c>
-      <c r="I16" s="24" t="s">
+      <c r="I18" s="24" t="s">
         <v>105</v>
       </c>
-      <c r="J16" s="25"/>
-    </row>
-    <row r="17" spans="2:10" ht="30">
-      <c r="B17" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="C17" s="49" t="s">
-        <v>102</v>
-      </c>
-      <c r="D17" s="20" t="s">
-        <v>108</v>
-      </c>
-      <c r="E17" s="21">
-        <v>42769</v>
-      </c>
-      <c r="F17" s="22" t="s">
-        <v>107</v>
-      </c>
-      <c r="G17" s="23" t="s">
-        <v>109</v>
-      </c>
-      <c r="H17" s="71" t="s">
-        <v>110</v>
-      </c>
-      <c r="I17" s="24" t="s">
-        <v>111</v>
-      </c>
-      <c r="J17" s="25"/>
-    </row>
-    <row r="18" spans="2:10" ht="30">
-      <c r="B18" s="56" t="s">
-        <v>37</v>
-      </c>
-      <c r="C18" s="57" t="s">
-        <v>102</v>
-      </c>
-      <c r="D18" s="94" t="s">
-        <v>102</v>
-      </c>
-      <c r="E18" s="59">
-        <v>42853</v>
-      </c>
-      <c r="F18" s="37" t="s">
-        <v>97</v>
-      </c>
-      <c r="G18" s="40" t="s">
-        <v>173</v>
-      </c>
-      <c r="H18" s="95" t="s">
-        <v>174</v>
-      </c>
-      <c r="I18" s="95" t="s">
-        <v>175</v>
-      </c>
-      <c r="J18" s="62"/>
-    </row>
-    <row r="19" spans="2:10" ht="45">
-      <c r="B19" s="56" t="s">
+      <c r="J18" s="25"/>
+    </row>
+    <row r="19" spans="2:10" ht="30">
+      <c r="B19" s="19" t="s">
         <v>37</v>
       </c>
       <c r="C19" s="49" t="s">
         <v>102</v>
       </c>
-      <c r="D19" s="101" t="s">
+      <c r="D19" s="20" t="s">
+        <v>108</v>
+      </c>
+      <c r="E19" s="21">
+        <v>42769</v>
+      </c>
+      <c r="F19" s="22" t="s">
+        <v>107</v>
+      </c>
+      <c r="G19" s="23" t="s">
+        <v>109</v>
+      </c>
+      <c r="H19" s="71" t="s">
+        <v>110</v>
+      </c>
+      <c r="I19" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="J19" s="25"/>
+    </row>
+    <row r="20" spans="2:10" ht="30">
+      <c r="B20" s="56" t="s">
+        <v>37</v>
+      </c>
+      <c r="C20" s="57" t="s">
         <v>102</v>
       </c>
-      <c r="E19" s="21">
-        <v>42898</v>
-      </c>
-      <c r="F19" s="93" t="s">
-        <v>107</v>
-      </c>
-      <c r="G19" s="91" t="s">
-        <v>208</v>
-      </c>
-      <c r="H19" s="71" t="s">
-        <v>210</v>
-      </c>
-      <c r="I19" s="71" t="s">
-        <v>209</v>
-      </c>
-      <c r="J19" s="25"/>
-    </row>
-    <row r="20" spans="2:10" ht="30" customHeight="1"/>
-    <row r="21" spans="2:10" ht="60">
+      <c r="D20" s="94" t="s">
+        <v>102</v>
+      </c>
+      <c r="E20" s="59">
+        <v>42853</v>
+      </c>
+      <c r="F20" s="37" t="s">
+        <v>97</v>
+      </c>
+      <c r="G20" s="40" t="s">
+        <v>173</v>
+      </c>
+      <c r="H20" s="95" t="s">
+        <v>174</v>
+      </c>
+      <c r="I20" s="95" t="s">
+        <v>175</v>
+      </c>
+      <c r="J20" s="62"/>
+    </row>
+    <row r="21" spans="2:10" ht="45">
       <c r="B21" s="56" t="s">
         <v>37</v>
       </c>
-      <c r="C21" s="57" t="s">
+      <c r="C21" s="49" t="s">
+        <v>102</v>
+      </c>
+      <c r="D21" s="101" t="s">
+        <v>102</v>
+      </c>
+      <c r="E21" s="21">
+        <v>42898</v>
+      </c>
+      <c r="F21" s="93" t="s">
+        <v>107</v>
+      </c>
+      <c r="G21" s="91" t="s">
+        <v>205</v>
+      </c>
+      <c r="H21" s="71" t="s">
+        <v>207</v>
+      </c>
+      <c r="I21" s="71" t="s">
+        <v>206</v>
+      </c>
+      <c r="J21" s="25"/>
+    </row>
+    <row r="22" spans="2:10" ht="30">
+      <c r="B22" s="56" t="s">
+        <v>37</v>
+      </c>
+      <c r="C22" s="49" t="s">
+        <v>102</v>
+      </c>
+      <c r="D22" s="101" t="s">
+        <v>102</v>
+      </c>
+      <c r="E22" s="21">
+        <v>43097</v>
+      </c>
+      <c r="F22" s="93" t="s">
+        <v>107</v>
+      </c>
+      <c r="G22" s="91" t="s">
+        <v>259</v>
+      </c>
+      <c r="H22" s="71" t="s">
+        <v>260</v>
+      </c>
+      <c r="I22" s="71" t="s">
+        <v>261</v>
+      </c>
+      <c r="J22" s="25"/>
+    </row>
+    <row r="23" spans="2:10" ht="30" customHeight="1"/>
+    <row r="24" spans="2:10" ht="60">
+      <c r="B24" s="56" t="s">
+        <v>37</v>
+      </c>
+      <c r="C24" s="57" t="s">
         <v>55</v>
       </c>
-      <c r="D21" s="58" t="s">
+      <c r="D24" s="58" t="s">
         <v>56</v>
       </c>
-      <c r="E21" s="59">
+      <c r="E24" s="59">
         <v>42741</v>
       </c>
-      <c r="F21" s="37" t="s">
+      <c r="F24" s="37" t="s">
         <v>97</v>
       </c>
-      <c r="G21" s="60" t="s">
+      <c r="G24" s="60" t="s">
         <v>57</v>
       </c>
-      <c r="H21" s="61" t="s">
+      <c r="H24" s="61" t="s">
         <v>116</v>
       </c>
-      <c r="I21" s="61" t="s">
+      <c r="I24" s="61" t="s">
         <v>58</v>
       </c>
-      <c r="J21" s="62"/>
-    </row>
-    <row r="22" spans="2:10" ht="45">
-      <c r="B22" s="19" t="s">
+      <c r="J24" s="62"/>
+    </row>
+    <row r="25" spans="2:10" ht="45">
+      <c r="B25" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="C22" s="49" t="s">
+      <c r="C25" s="49" t="s">
         <v>55</v>
       </c>
-      <c r="D22" s="20" t="s">
+      <c r="D25" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="E22" s="21">
+      <c r="E25" s="21">
         <v>42745</v>
       </c>
-      <c r="F22" s="22" t="s">
+      <c r="F25" s="22" t="s">
         <v>107</v>
       </c>
-      <c r="G22" s="23" t="s">
+      <c r="G25" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="H22" s="24" t="s">
+      <c r="H25" s="24" t="s">
         <v>117</v>
       </c>
-      <c r="I22" s="24" t="s">
+      <c r="I25" s="24" t="s">
         <v>118</v>
       </c>
-      <c r="J22" s="25"/>
-    </row>
-    <row r="23" spans="2:10" ht="30">
-      <c r="B23" s="26" t="s">
+      <c r="J25" s="25"/>
+    </row>
+    <row r="26" spans="2:10" ht="30">
+      <c r="B26" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="C23" s="51" t="s">
+      <c r="C26" s="51" t="s">
         <v>55</v>
       </c>
-      <c r="D23" s="27"/>
-      <c r="E23" s="28">
+      <c r="D26" s="27"/>
+      <c r="E26" s="28">
         <v>42745</v>
       </c>
-      <c r="F23" s="29" t="s">
+      <c r="F26" s="29" t="s">
         <v>98</v>
       </c>
-      <c r="G23" s="27" t="s">
+      <c r="G26" s="27" t="s">
         <v>66</v>
       </c>
-      <c r="H23" s="31" t="s">
+      <c r="H26" s="31" t="s">
         <v>67</v>
       </c>
-      <c r="I23" s="31"/>
-      <c r="J23" s="32"/>
-    </row>
-    <row r="24" spans="2:10" ht="30">
-      <c r="B24" s="26" t="s">
+      <c r="I26" s="31"/>
+      <c r="J26" s="32"/>
+    </row>
+    <row r="27" spans="2:10" ht="30">
+      <c r="B27" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="C24" s="51" t="s">
+      <c r="C27" s="51" t="s">
         <v>55</v>
       </c>
-      <c r="D24" s="27"/>
-      <c r="E24" s="28">
+      <c r="D27" s="27"/>
+      <c r="E27" s="28">
         <v>42793</v>
       </c>
-      <c r="F24" s="29" t="s">
+      <c r="F27" s="29" t="s">
         <v>98</v>
       </c>
-      <c r="G24" s="27" t="s">
+      <c r="G27" s="27" t="s">
         <v>140</v>
       </c>
-      <c r="H24" s="31" t="s">
+      <c r="H27" s="31" t="s">
         <v>141</v>
       </c>
-      <c r="I24" s="31" t="s">
+      <c r="I27" s="31" t="s">
         <v>142</v>
       </c>
-      <c r="J24" s="32"/>
-    </row>
-    <row r="25" spans="2:10" ht="30">
-      <c r="B25" s="26" t="s">
+      <c r="J27" s="32"/>
+    </row>
+    <row r="28" spans="2:10" ht="30">
+      <c r="B28" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="C25" s="51" t="s">
+      <c r="C28" s="51" t="s">
         <v>55</v>
       </c>
-      <c r="D25" s="27"/>
-      <c r="E25" s="28">
+      <c r="D28" s="27"/>
+      <c r="E28" s="28">
         <v>42802</v>
       </c>
-      <c r="F25" s="29" t="s">
+      <c r="F28" s="29" t="s">
         <v>98</v>
       </c>
-      <c r="G25" s="27" t="s">
+      <c r="G28" s="27" t="s">
         <v>148</v>
       </c>
-      <c r="H25" s="31" t="s">
+      <c r="H28" s="31" t="s">
         <v>149</v>
       </c>
-      <c r="I25" s="31" t="s">
+      <c r="I28" s="31" t="s">
         <v>150</v>
       </c>
-      <c r="J25" s="32"/>
-    </row>
-    <row r="26" spans="2:10" ht="30">
-      <c r="B26" s="19" t="s">
+      <c r="J28" s="32"/>
+    </row>
+    <row r="29" spans="2:10" ht="30">
+      <c r="B29" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="C26" s="49" t="s">
+      <c r="C29" s="49" t="s">
         <v>55</v>
       </c>
-      <c r="D26" s="20" t="s">
+      <c r="D29" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="E26" s="21">
+      <c r="E29" s="21">
         <v>42839</v>
       </c>
-      <c r="F26" s="22" t="s">
+      <c r="F29" s="22" t="s">
         <v>107</v>
       </c>
-      <c r="G26" s="91" t="s">
+      <c r="G29" s="91" t="s">
         <v>165</v>
       </c>
-      <c r="H26" s="71" t="s">
+      <c r="H29" s="71" t="s">
         <v>163</v>
       </c>
-      <c r="I26" s="71" t="s">
+      <c r="I29" s="71" t="s">
         <v>164</v>
       </c>
-      <c r="J26" s="25"/>
-    </row>
-    <row r="27" spans="2:10" ht="15.75">
-      <c r="B27" s="19" t="s">
+      <c r="J29" s="25"/>
+    </row>
+    <row r="30" spans="2:10" ht="15.75">
+      <c r="B30" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="C27" s="49" t="s">
+      <c r="C30" s="49" t="s">
         <v>55</v>
       </c>
-      <c r="D27" s="20" t="s">
+      <c r="D30" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="E27" s="21">
+      <c r="E30" s="21">
         <v>43053</v>
       </c>
-      <c r="F27" s="22" t="s">
+      <c r="F30" s="22" t="s">
         <v>107</v>
       </c>
-      <c r="G27" s="91" t="s">
+      <c r="G30" s="91" t="s">
+        <v>250</v>
+      </c>
+      <c r="H30" s="71" t="s">
+        <v>251</v>
+      </c>
+      <c r="I30" s="71" t="s">
+        <v>252</v>
+      </c>
+      <c r="J30" s="25"/>
+    </row>
+    <row r="31" spans="2:10" ht="60">
+      <c r="B31" s="56" t="s">
+        <v>37</v>
+      </c>
+      <c r="C31" s="57" t="s">
+        <v>55</v>
+      </c>
+      <c r="D31" s="58" t="s">
+        <v>56</v>
+      </c>
+      <c r="E31" s="59">
+        <v>43080</v>
+      </c>
+      <c r="F31" s="37" t="s">
+        <v>97</v>
+      </c>
+      <c r="G31" s="40" t="s">
         <v>253</v>
       </c>
-      <c r="H27" s="71" t="s">
+      <c r="H31" s="95" t="s">
         <v>254</v>
       </c>
-      <c r="I27" s="71" t="s">
+      <c r="I31" s="95" t="s">
         <v>255</v>
       </c>
-      <c r="J27" s="25"/>
-    </row>
-    <row r="28" spans="2:10" ht="30" customHeight="1"/>
-    <row r="29" spans="2:10" ht="38.25" customHeight="1">
-      <c r="B29" s="92" t="s">
+      <c r="J31" s="62"/>
+    </row>
+    <row r="32" spans="2:10" ht="30" customHeight="1"/>
+    <row r="33" spans="2:10" ht="38.25" customHeight="1">
+      <c r="B33" s="92" t="s">
         <v>37</v>
       </c>
-      <c r="C29" s="57" t="s">
+      <c r="C33" s="57" t="s">
         <v>166</v>
       </c>
-      <c r="D29" s="92"/>
-      <c r="E29" s="92">
+      <c r="D33" s="92"/>
+      <c r="E33" s="92">
         <v>42826</v>
       </c>
-      <c r="F29" s="92" t="s">
+      <c r="F33" s="92" t="s">
         <v>97</v>
       </c>
-      <c r="G29" s="92" t="s">
+      <c r="G33" s="92" t="s">
         <v>167</v>
       </c>
-      <c r="H29" s="96" t="s">
-        <v>206</v>
-      </c>
-      <c r="I29" s="92"/>
-      <c r="J29" s="92"/>
-    </row>
-    <row r="30" spans="2:10" ht="60">
-      <c r="B30" s="103" t="s">
+      <c r="H33" s="96" t="s">
+        <v>203</v>
+      </c>
+      <c r="I33" s="92"/>
+      <c r="J33" s="92"/>
+    </row>
+    <row r="34" spans="2:10" ht="60">
+      <c r="B34" s="103" t="s">
         <v>37</v>
       </c>
-      <c r="C30" s="49" t="s">
+      <c r="C34" s="49" t="s">
         <v>166</v>
       </c>
-      <c r="D30" s="101" t="s">
-        <v>224</v>
-      </c>
-      <c r="E30" s="21">
+      <c r="D34" s="101" t="s">
+        <v>221</v>
+      </c>
+      <c r="E34" s="21">
         <v>42996</v>
       </c>
-      <c r="F30" s="93" t="s">
+      <c r="F34" s="93" t="s">
         <v>107</v>
       </c>
-      <c r="G30" s="106" t="s">
-        <v>218</v>
-      </c>
-      <c r="H30" s="71" t="s">
-        <v>225</v>
-      </c>
-      <c r="I30" s="71" t="s">
-        <v>226</v>
-      </c>
-      <c r="J30" s="67"/>
-    </row>
-    <row r="31" spans="2:10" ht="30">
-      <c r="B31" s="107" t="s">
+      <c r="G34" s="106" t="s">
+        <v>215</v>
+      </c>
+      <c r="H34" s="71" t="s">
+        <v>222</v>
+      </c>
+      <c r="I34" s="71" t="s">
+        <v>223</v>
+      </c>
+      <c r="J34" s="67"/>
+    </row>
+    <row r="35" spans="2:10" ht="30">
+      <c r="B35" s="107" t="s">
         <v>37</v>
       </c>
-      <c r="C31" s="73" t="s">
+      <c r="C35" s="73" t="s">
         <v>166</v>
       </c>
-      <c r="D31" s="87" t="s">
-        <v>224</v>
-      </c>
-      <c r="E31" s="75">
+      <c r="D35" s="87" t="s">
+        <v>221</v>
+      </c>
+      <c r="E35" s="75">
         <v>43023</v>
-      </c>
-      <c r="F31" s="29" t="s">
-        <v>98</v>
-      </c>
-      <c r="G31" s="102" t="s">
-        <v>236</v>
-      </c>
-      <c r="H31" s="78" t="s">
-        <v>237</v>
-      </c>
-      <c r="I31" s="78" t="s">
-        <v>238</v>
-      </c>
-      <c r="J31" s="77"/>
-    </row>
-    <row r="32" spans="2:10" ht="30">
-      <c r="B32" s="103" t="s">
-        <v>37</v>
-      </c>
-      <c r="C32" s="49" t="s">
-        <v>166</v>
-      </c>
-      <c r="D32" s="101" t="s">
-        <v>242</v>
-      </c>
-      <c r="E32" s="21">
-        <v>43047</v>
-      </c>
-      <c r="F32" s="93" t="s">
-        <v>107</v>
-      </c>
-      <c r="G32" s="106" t="s">
-        <v>243</v>
-      </c>
-      <c r="H32" s="71" t="s">
-        <v>244</v>
-      </c>
-      <c r="I32" s="71" t="s">
-        <v>248</v>
-      </c>
-      <c r="J32" s="67"/>
-    </row>
-    <row r="33" spans="2:10" ht="45">
-      <c r="B33" s="103" t="s">
-        <v>37</v>
-      </c>
-      <c r="C33" s="49" t="s">
-        <v>166</v>
-      </c>
-      <c r="D33" s="101" t="s">
-        <v>242</v>
-      </c>
-      <c r="E33" s="21">
-        <v>43047</v>
-      </c>
-      <c r="F33" s="93" t="s">
-        <v>107</v>
-      </c>
-      <c r="G33" s="106" t="s">
-        <v>246</v>
-      </c>
-      <c r="H33" s="71" t="s">
-        <v>247</v>
-      </c>
-      <c r="I33" s="71" t="s">
-        <v>245</v>
-      </c>
-      <c r="J33" s="67"/>
-    </row>
-    <row r="34" spans="2:10" ht="30" customHeight="1"/>
-    <row r="35" spans="2:10" ht="45">
-      <c r="B35" s="26" t="s">
-        <v>37</v>
-      </c>
-      <c r="C35" s="51" t="s">
-        <v>81</v>
-      </c>
-      <c r="D35" s="27" t="s">
-        <v>85</v>
-      </c>
-      <c r="E35" s="28">
-        <v>42750</v>
       </c>
       <c r="F35" s="29" t="s">
         <v>98</v>
       </c>
-      <c r="G35" s="27" t="s">
+      <c r="G35" s="102" t="s">
+        <v>233</v>
+      </c>
+      <c r="H35" s="78" t="s">
+        <v>234</v>
+      </c>
+      <c r="I35" s="78" t="s">
+        <v>235</v>
+      </c>
+      <c r="J35" s="77"/>
+    </row>
+    <row r="36" spans="2:10" ht="30">
+      <c r="B36" s="103" t="s">
+        <v>37</v>
+      </c>
+      <c r="C36" s="49" t="s">
+        <v>166</v>
+      </c>
+      <c r="D36" s="101" t="s">
+        <v>239</v>
+      </c>
+      <c r="E36" s="21">
+        <v>43047</v>
+      </c>
+      <c r="F36" s="93" t="s">
+        <v>107</v>
+      </c>
+      <c r="G36" s="106" t="s">
+        <v>240</v>
+      </c>
+      <c r="H36" s="71" t="s">
+        <v>241</v>
+      </c>
+      <c r="I36" s="71" t="s">
+        <v>245</v>
+      </c>
+      <c r="J36" s="67"/>
+    </row>
+    <row r="37" spans="2:10" ht="45">
+      <c r="B37" s="103" t="s">
+        <v>37</v>
+      </c>
+      <c r="C37" s="49" t="s">
+        <v>166</v>
+      </c>
+      <c r="D37" s="101" t="s">
+        <v>239</v>
+      </c>
+      <c r="E37" s="21">
+        <v>43047</v>
+      </c>
+      <c r="F37" s="93" t="s">
+        <v>107</v>
+      </c>
+      <c r="G37" s="106" t="s">
+        <v>243</v>
+      </c>
+      <c r="H37" s="71" t="s">
+        <v>244</v>
+      </c>
+      <c r="I37" s="71" t="s">
+        <v>242</v>
+      </c>
+      <c r="J37" s="67"/>
+    </row>
+    <row r="38" spans="2:10" ht="29.25" customHeight="1"/>
+    <row r="39" spans="2:10" ht="30">
+      <c r="B39" s="72" t="s">
+        <v>37</v>
+      </c>
+      <c r="C39" s="73" t="s">
+        <v>266</v>
+      </c>
+      <c r="D39" s="87" t="s">
+        <v>267</v>
+      </c>
+      <c r="E39" s="75">
+        <v>43110</v>
+      </c>
+      <c r="F39" s="29" t="s">
+        <v>98</v>
+      </c>
+      <c r="G39" s="30" t="s">
+        <v>268</v>
+      </c>
+      <c r="H39" s="78" t="s">
+        <v>269</v>
+      </c>
+      <c r="I39" s="78"/>
+      <c r="J39" s="108"/>
+    </row>
+    <row r="40" spans="2:10" ht="30" customHeight="1"/>
+    <row r="41" spans="2:10" ht="45">
+      <c r="B41" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="C41" s="51" t="s">
+        <v>81</v>
+      </c>
+      <c r="D41" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="E41" s="28">
+        <v>42750</v>
+      </c>
+      <c r="F41" s="29" t="s">
+        <v>98</v>
+      </c>
+      <c r="G41" s="27" t="s">
         <v>83</v>
       </c>
-      <c r="H35" s="31" t="s">
+      <c r="H41" s="31" t="s">
         <v>84</v>
       </c>
-      <c r="I35" s="31"/>
-      <c r="J35" s="32"/>
-    </row>
-    <row r="36" spans="2:10" ht="60">
-      <c r="B36" s="26" t="s">
+      <c r="I41" s="31"/>
+      <c r="J41" s="32"/>
+    </row>
+    <row r="42" spans="2:10" ht="60">
+      <c r="B42" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="C36" s="51" t="s">
+      <c r="C42" s="51" t="s">
         <v>81</v>
       </c>
-      <c r="D36" s="27" t="s">
+      <c r="D42" s="27" t="s">
         <v>85</v>
       </c>
-      <c r="E36" s="28">
+      <c r="E42" s="28">
         <v>42750</v>
       </c>
-      <c r="F36" s="29" t="s">
+      <c r="F42" s="29" t="s">
         <v>98</v>
       </c>
-      <c r="G36" s="30" t="s">
+      <c r="G42" s="30" t="s">
         <v>82</v>
       </c>
-      <c r="H36" s="31" t="s">
+      <c r="H42" s="31" t="s">
         <v>79</v>
       </c>
-      <c r="I36" s="31" t="s">
+      <c r="I42" s="31" t="s">
         <v>80</v>
       </c>
-      <c r="J36" s="32"/>
-    </row>
-    <row r="37" spans="2:10" ht="30">
-      <c r="B37" s="26" t="s">
+      <c r="J42" s="32"/>
+    </row>
+    <row r="43" spans="2:10" ht="30">
+      <c r="B43" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="C37" s="51" t="s">
+      <c r="C43" s="51" t="s">
         <v>81</v>
       </c>
-      <c r="D37" s="27" t="s">
+      <c r="D43" s="27" t="s">
         <v>86</v>
       </c>
-      <c r="E37" s="28">
+      <c r="E43" s="28">
         <v>42750</v>
       </c>
-      <c r="F37" s="29" t="s">
+      <c r="F43" s="29" t="s">
         <v>98</v>
       </c>
-      <c r="G37" s="30" t="s">
+      <c r="G43" s="30" t="s">
         <v>87</v>
       </c>
-      <c r="H37" s="31" t="s">
+      <c r="H43" s="31" t="s">
         <v>88</v>
       </c>
-      <c r="I37" s="31" t="s">
+      <c r="I43" s="31" t="s">
         <v>89</v>
       </c>
-      <c r="J37" s="32"/>
+      <c r="J43" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
!U PPC updates for our internal parentSpace management in the puppet rigs
</commit_message>
<xml_diff>
--- a/Codebase_Tracker.xlsx
+++ b/Codebase_Tracker.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="292">
   <si>
     <t>Module</t>
   </si>
@@ -865,6 +865,33 @@
   </si>
   <si>
     <t>!!</t>
+  </si>
+  <si>
+    <t>Added direct exposure of the animPointCloud to the Pro_MetaRig so that we can use it to transpose world space on the fly</t>
+  </si>
+  <si>
+    <t>this isn't yet exposed except in code but is a really key function to allow us to change data on the fly without it effecting the rigs pose</t>
+  </si>
+  <si>
+    <t>anim_point_cloud  - code</t>
+  </si>
+  <si>
+    <t>switch_attr_compensated - code</t>
+  </si>
+  <si>
+    <t>a wrapper over the anim_point_cloud, allowing an attribute on a node to be changed whilst compensating for that change in the rigs transforms</t>
+  </si>
+  <si>
+    <t>this will eventually be exposed to allow us to change Parent spaces on the fly, both static and over time</t>
+  </si>
+  <si>
+    <t>ik_fk_match, fk_ik_match</t>
+  </si>
+  <si>
+    <t>new timerange flag added to allow us to directly pass in the timerange to process</t>
+  </si>
+  <si>
+    <t>previously time was just a bool which triggered a get of the current timeline bounds only</t>
   </si>
 </sst>
 </file>
@@ -1060,7 +1087,7 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="118">
+  <cellXfs count="121">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1407,11 +1434,20 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="4" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="4" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="4" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="4" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="4" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -1726,10 +1762,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:M69"/>
+  <dimension ref="A2:M72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="D58" sqref="D58"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="G45" sqref="G45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1748,17 +1784,17 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:13" ht="21">
-      <c r="B2" s="116" t="s">
+      <c r="B2" s="117" t="s">
         <v>137</v>
       </c>
-      <c r="C2" s="116"/>
-      <c r="D2" s="116"/>
-      <c r="E2" s="116"/>
-      <c r="F2" s="116"/>
-      <c r="G2" s="116"/>
-      <c r="H2" s="116"/>
-      <c r="I2" s="116"/>
-      <c r="J2" s="116"/>
+      <c r="C2" s="117"/>
+      <c r="D2" s="117"/>
+      <c r="E2" s="117"/>
+      <c r="F2" s="117"/>
+      <c r="G2" s="117"/>
+      <c r="H2" s="117"/>
+      <c r="I2" s="117"/>
+      <c r="J2" s="117"/>
     </row>
     <row r="3" spans="1:13" ht="15.6" customHeight="1"/>
     <row r="4" spans="1:13" s="2" customFormat="1" ht="24" customHeight="1">
@@ -2610,7 +2646,7 @@
       <c r="I39" s="31"/>
       <c r="J39" s="68"/>
     </row>
-    <row r="40" spans="2:10" ht="15.75">
+    <row r="40" spans="2:10" ht="21" customHeight="1">
       <c r="B40" s="26" t="s">
         <v>16</v>
       </c>
@@ -2743,231 +2779,252 @@
       </c>
       <c r="J44" s="112"/>
     </row>
-    <row r="45" spans="2:10" ht="30" customHeight="1">
-      <c r="C45" s="52"/>
-      <c r="F45" s="6"/>
-      <c r="G45" s="7"/>
-      <c r="H45" s="11"/>
-    </row>
-    <row r="46" spans="2:10" ht="60">
-      <c r="B46" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="C46" s="49" t="s">
+    <row r="45" spans="2:10" ht="45">
+      <c r="B45" s="118" t="s">
+        <v>16</v>
+      </c>
+      <c r="C45" s="119" t="s">
+        <v>17</v>
+      </c>
+      <c r="D45" s="119" t="s">
+        <v>41</v>
+      </c>
+      <c r="E45" s="75">
+        <v>43154</v>
+      </c>
+      <c r="F45" s="29" t="s">
+        <v>98</v>
+      </c>
+      <c r="G45" s="30" t="s">
+        <v>285</v>
+      </c>
+      <c r="H45" s="31" t="s">
+        <v>283</v>
+      </c>
+      <c r="I45" s="31" t="s">
+        <v>284</v>
+      </c>
+      <c r="J45" s="120"/>
+    </row>
+    <row r="46" spans="2:10" ht="45">
+      <c r="B46" s="118" t="s">
+        <v>16</v>
+      </c>
+      <c r="C46" s="119" t="s">
+        <v>17</v>
+      </c>
+      <c r="D46" s="119" t="s">
+        <v>41</v>
+      </c>
+      <c r="E46" s="75">
+        <v>43154</v>
+      </c>
+      <c r="F46" s="29" t="s">
+        <v>98</v>
+      </c>
+      <c r="G46" s="30" t="s">
+        <v>286</v>
+      </c>
+      <c r="H46" s="31" t="s">
+        <v>287</v>
+      </c>
+      <c r="I46" s="31" t="s">
+        <v>288</v>
+      </c>
+      <c r="J46" s="120"/>
+    </row>
+    <row r="47" spans="2:10" ht="30">
+      <c r="B47" s="118" t="s">
+        <v>16</v>
+      </c>
+      <c r="C47" s="119" t="s">
+        <v>17</v>
+      </c>
+      <c r="D47" s="119" t="s">
+        <v>41</v>
+      </c>
+      <c r="E47" s="75">
+        <v>43154</v>
+      </c>
+      <c r="F47" s="29" t="s">
+        <v>98</v>
+      </c>
+      <c r="G47" s="30" t="s">
+        <v>289</v>
+      </c>
+      <c r="H47" s="31" t="s">
+        <v>290</v>
+      </c>
+      <c r="I47" s="31" t="s">
+        <v>291</v>
+      </c>
+      <c r="J47" s="120"/>
+    </row>
+    <row r="48" spans="2:10" ht="30" customHeight="1">
+      <c r="C48" s="52"/>
+      <c r="F48" s="6"/>
+      <c r="G48" s="7"/>
+      <c r="H48" s="11"/>
+    </row>
+    <row r="49" spans="1:10" ht="60">
+      <c r="B49" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="C49" s="49" t="s">
         <v>13</v>
       </c>
-      <c r="D46" s="20" t="s">
+      <c r="D49" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="E46" s="21">
+      <c r="E49" s="21">
         <v>42734</v>
       </c>
-      <c r="F46" s="22" t="s">
+      <c r="F49" s="22" t="s">
         <v>107</v>
       </c>
-      <c r="G46" s="23" t="s">
+      <c r="G49" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="H46" s="24" t="s">
+      <c r="H49" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="I46" s="24" t="s">
+      <c r="I49" s="24" t="s">
         <v>132</v>
       </c>
-      <c r="J46" s="67"/>
-    </row>
-    <row r="47" spans="2:10" ht="45">
-      <c r="B47" s="34" t="s">
-        <v>16</v>
-      </c>
-      <c r="C47" s="50" t="s">
+      <c r="J49" s="67"/>
+    </row>
+    <row r="50" spans="1:10" ht="45">
+      <c r="B50" s="34" t="s">
+        <v>16</v>
+      </c>
+      <c r="C50" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="D47" s="35" t="s">
+      <c r="D50" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="E47" s="36">
+      <c r="E50" s="36">
         <v>42740</v>
       </c>
-      <c r="F47" s="37" t="s">
+      <c r="F50" s="37" t="s">
         <v>97</v>
       </c>
-      <c r="G47" s="40" t="s">
+      <c r="G50" s="40" t="s">
         <v>75</v>
       </c>
-      <c r="H47" s="38" t="s">
+      <c r="H50" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="I47" s="35"/>
-      <c r="J47" s="66"/>
-    </row>
-    <row r="48" spans="2:10" ht="45">
-      <c r="B48" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="C48" s="49" t="s">
+      <c r="I50" s="35"/>
+      <c r="J50" s="66"/>
+    </row>
+    <row r="51" spans="1:10" ht="45">
+      <c r="B51" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="C51" s="49" t="s">
         <v>13</v>
       </c>
-      <c r="D48" s="20" t="s">
+      <c r="D51" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="E48" s="21">
+      <c r="E51" s="21">
         <v>42745</v>
       </c>
-      <c r="F48" s="22" t="s">
+      <c r="F51" s="22" t="s">
         <v>107</v>
       </c>
-      <c r="G48" s="23" t="s">
+      <c r="G51" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="H48" s="24" t="s">
+      <c r="H51" s="24" t="s">
         <v>64</v>
       </c>
-      <c r="I48" s="20" t="s">
+      <c r="I51" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="J48" s="67"/>
-    </row>
-    <row r="49" spans="1:10" ht="45">
-      <c r="B49" s="79" t="s">
-        <v>16</v>
-      </c>
-      <c r="C49" s="80" t="s">
+      <c r="J51" s="67"/>
+    </row>
+    <row r="52" spans="1:10" ht="45">
+      <c r="B52" s="79" t="s">
+        <v>16</v>
+      </c>
+      <c r="C52" s="80" t="s">
         <v>13</v>
       </c>
-      <c r="D49" s="83" t="s">
+      <c r="D52" s="83" t="s">
         <v>13</v>
       </c>
-      <c r="E49" s="81">
+      <c r="E52" s="81">
         <v>42811</v>
       </c>
-      <c r="F49" s="13" t="s">
+      <c r="F52" s="13" t="s">
         <v>136</v>
       </c>
-      <c r="G49" s="46" t="s">
+      <c r="G52" s="46" t="s">
         <v>151</v>
       </c>
-      <c r="H49" s="84" t="s">
+      <c r="H52" s="84" t="s">
         <v>152</v>
       </c>
-      <c r="I49" s="83" t="s">
+      <c r="I52" s="83" t="s">
         <v>153</v>
       </c>
-      <c r="J49" s="82"/>
-    </row>
-    <row r="50" spans="1:10" ht="45">
-      <c r="B50" s="86" t="s">
-        <v>16</v>
-      </c>
-      <c r="C50" s="73" t="s">
+      <c r="J52" s="82"/>
+    </row>
+    <row r="53" spans="1:10" ht="45">
+      <c r="B53" s="86" t="s">
+        <v>16</v>
+      </c>
+      <c r="C53" s="73" t="s">
         <v>13</v>
       </c>
-      <c r="D50" s="87" t="s">
+      <c r="D53" s="87" t="s">
         <v>13</v>
       </c>
-      <c r="E50" s="88">
+      <c r="E53" s="88">
         <v>42817</v>
       </c>
-      <c r="F50" s="89" t="s">
+      <c r="F53" s="89" t="s">
         <v>98</v>
       </c>
-      <c r="G50" s="30" t="s">
+      <c r="G53" s="30" t="s">
         <v>151</v>
       </c>
-      <c r="H50" s="78" t="s">
+      <c r="H53" s="78" t="s">
         <v>161</v>
       </c>
-      <c r="I50" s="78" t="s">
+      <c r="I53" s="78" t="s">
         <v>162</v>
       </c>
-      <c r="J50" s="90"/>
-    </row>
-    <row r="51" spans="1:10" ht="30">
-      <c r="B51" s="86" t="s">
-        <v>16</v>
-      </c>
-      <c r="C51" s="73" t="s">
+      <c r="J53" s="90"/>
+    </row>
+    <row r="54" spans="1:10" ht="30">
+      <c r="B54" s="86" t="s">
+        <v>16</v>
+      </c>
+      <c r="C54" s="73" t="s">
         <v>13</v>
       </c>
-      <c r="D51" s="87" t="s">
+      <c r="D54" s="87" t="s">
         <v>13</v>
       </c>
-      <c r="E51" s="88">
+      <c r="E54" s="88">
         <v>43110</v>
       </c>
-      <c r="F51" s="89" t="s">
+      <c r="F54" s="89" t="s">
         <v>98</v>
       </c>
-      <c r="G51" s="30" t="s">
+      <c r="G54" s="30" t="s">
         <v>151</v>
       </c>
-      <c r="H51" s="78" t="s">
+      <c r="H54" s="78" t="s">
         <v>273</v>
       </c>
-      <c r="I51" s="78" t="s">
+      <c r="I54" s="78" t="s">
         <v>274</v>
       </c>
-      <c r="J51" s="90"/>
-    </row>
-    <row r="52" spans="1:10" ht="30" customHeight="1">
-      <c r="C52" s="52"/>
-      <c r="F52" s="6"/>
-      <c r="G52" s="7"/>
-      <c r="H52" s="11"/>
-    </row>
-    <row r="53" spans="1:10" ht="30">
-      <c r="B53" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="C53" s="49" t="s">
-        <v>119</v>
-      </c>
-      <c r="D53" s="20" t="s">
-        <v>120</v>
-      </c>
-      <c r="E53" s="21">
-        <v>42745</v>
-      </c>
-      <c r="F53" s="22" t="s">
-        <v>107</v>
-      </c>
-      <c r="G53" s="23" t="s">
-        <v>121</v>
-      </c>
-      <c r="H53" s="24" t="s">
-        <v>122</v>
-      </c>
-      <c r="I53" s="20" t="s">
-        <v>123</v>
-      </c>
-      <c r="J53" s="67"/>
-    </row>
-    <row r="54" spans="1:10" ht="60">
-      <c r="B54" s="72" t="s">
-        <v>16</v>
-      </c>
-      <c r="C54" s="73" t="s">
-        <v>119</v>
-      </c>
-      <c r="D54" s="87" t="s">
-        <v>187</v>
-      </c>
-      <c r="E54" s="75">
-        <v>43110</v>
-      </c>
-      <c r="F54" s="29" t="s">
-        <v>97</v>
-      </c>
-      <c r="G54" s="30" t="s">
-        <v>270</v>
-      </c>
-      <c r="H54" s="78" t="s">
-        <v>271</v>
-      </c>
-      <c r="I54" s="78" t="s">
-        <v>272</v>
-      </c>
-      <c r="J54" s="77"/>
+      <c r="J54" s="90"/>
     </row>
     <row r="55" spans="1:10" ht="30" customHeight="1">
       <c r="C55" s="52"/>
@@ -2975,314 +3032,374 @@
       <c r="G55" s="7"/>
       <c r="H55" s="11"/>
     </row>
-    <row r="56" spans="1:10" ht="45">
+    <row r="56" spans="1:10" ht="30">
       <c r="B56" s="19" t="s">
         <v>16</v>
       </c>
       <c r="C56" s="49" t="s">
-        <v>18</v>
+        <v>119</v>
       </c>
       <c r="D56" s="20" t="s">
-        <v>14</v>
+        <v>120</v>
       </c>
       <c r="E56" s="21">
-        <v>42734</v>
+        <v>42745</v>
       </c>
       <c r="F56" s="22" t="s">
         <v>107</v>
       </c>
-      <c r="G56" s="23"/>
+      <c r="G56" s="23" t="s">
+        <v>121</v>
+      </c>
       <c r="H56" s="24" t="s">
+        <v>122</v>
+      </c>
+      <c r="I56" s="20" t="s">
+        <v>123</v>
+      </c>
+      <c r="J56" s="67"/>
+    </row>
+    <row r="57" spans="1:10" ht="60">
+      <c r="B57" s="72" t="s">
+        <v>16</v>
+      </c>
+      <c r="C57" s="73" t="s">
+        <v>119</v>
+      </c>
+      <c r="D57" s="87" t="s">
+        <v>187</v>
+      </c>
+      <c r="E57" s="75">
+        <v>43110</v>
+      </c>
+      <c r="F57" s="29" t="s">
+        <v>97</v>
+      </c>
+      <c r="G57" s="30" t="s">
+        <v>270</v>
+      </c>
+      <c r="H57" s="78" t="s">
+        <v>271</v>
+      </c>
+      <c r="I57" s="78" t="s">
+        <v>272</v>
+      </c>
+      <c r="J57" s="77"/>
+    </row>
+    <row r="58" spans="1:10" ht="30" customHeight="1">
+      <c r="C58" s="52"/>
+      <c r="F58" s="6"/>
+      <c r="G58" s="7"/>
+      <c r="H58" s="11"/>
+    </row>
+    <row r="59" spans="1:10" ht="45">
+      <c r="B59" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="C59" s="49" t="s">
+        <v>18</v>
+      </c>
+      <c r="D59" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="E59" s="21">
+        <v>42734</v>
+      </c>
+      <c r="F59" s="22" t="s">
+        <v>107</v>
+      </c>
+      <c r="G59" s="23"/>
+      <c r="H59" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="I56" s="20"/>
-      <c r="J56" s="67"/>
-    </row>
-    <row r="57" spans="1:10" ht="45">
-      <c r="B57" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="C57" s="49" t="s">
+      <c r="I59" s="20"/>
+      <c r="J59" s="67"/>
+    </row>
+    <row r="60" spans="1:10" ht="45">
+      <c r="B60" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="C60" s="49" t="s">
         <v>18</v>
       </c>
-      <c r="D57" s="20" t="s">
+      <c r="D60" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="E57" s="21">
+      <c r="E60" s="21">
         <v>42734</v>
       </c>
-      <c r="F57" s="93" t="s">
+      <c r="F60" s="93" t="s">
         <v>107</v>
       </c>
-      <c r="G57" s="23"/>
-      <c r="H57" s="24" t="s">
+      <c r="G60" s="23"/>
+      <c r="H60" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="I57" s="20"/>
-      <c r="J57" s="67"/>
-    </row>
-    <row r="58" spans="1:10" ht="75">
-      <c r="A58" s="115" t="s">
+      <c r="I60" s="20"/>
+      <c r="J60" s="67"/>
+    </row>
+    <row r="61" spans="1:10" ht="75">
+      <c r="A61" s="115" t="s">
         <v>282</v>
       </c>
-      <c r="B58" s="72" t="s">
-        <v>16</v>
-      </c>
-      <c r="C58" s="117" t="s">
+      <c r="B61" s="72" t="s">
+        <v>16</v>
+      </c>
+      <c r="C61" s="116" t="s">
         <v>18</v>
       </c>
-      <c r="D58" s="74" t="s">
+      <c r="D61" s="74" t="s">
         <v>14</v>
       </c>
-      <c r="E58" s="75">
+      <c r="E61" s="75">
         <v>43110</v>
       </c>
-      <c r="F58" s="113" t="s">
+      <c r="F61" s="113" t="s">
         <v>97</v>
       </c>
-      <c r="G58" s="76" t="s">
+      <c r="G61" s="76" t="s">
         <v>279</v>
       </c>
-      <c r="H58" s="114" t="s">
+      <c r="H61" s="114" t="s">
         <v>280</v>
       </c>
-      <c r="I58" s="74" t="s">
+      <c r="I61" s="74" t="s">
         <v>281</v>
       </c>
-      <c r="J58" s="77"/>
-    </row>
-    <row r="59" spans="1:10" ht="30" customHeight="1">
-      <c r="C59" s="52"/>
-      <c r="F59" s="6"/>
-      <c r="G59" s="7"/>
-      <c r="H59" s="11"/>
-    </row>
-    <row r="60" spans="1:10" ht="60">
-      <c r="B60" s="43" t="s">
-        <v>16</v>
-      </c>
-      <c r="C60" s="55" t="s">
+      <c r="J61" s="77"/>
+    </row>
+    <row r="62" spans="1:10" ht="30" customHeight="1">
+      <c r="C62" s="52"/>
+      <c r="F62" s="6"/>
+      <c r="G62" s="7"/>
+      <c r="H62" s="11"/>
+    </row>
+    <row r="63" spans="1:10" ht="60">
+      <c r="B63" s="43" t="s">
+        <v>16</v>
+      </c>
+      <c r="C63" s="55" t="s">
         <v>20</v>
       </c>
-      <c r="D60" s="33"/>
-      <c r="E60" s="44">
+      <c r="D63" s="33"/>
+      <c r="E63" s="44">
         <v>42709</v>
       </c>
-      <c r="F60" s="45" t="s">
+      <c r="F63" s="45" t="s">
         <v>98</v>
       </c>
-      <c r="G60" s="46"/>
-      <c r="H60" s="47" t="s">
+      <c r="G63" s="46"/>
+      <c r="H63" s="47" t="s">
         <v>21</v>
       </c>
-      <c r="I60" s="47" t="s">
+      <c r="I63" s="47" t="s">
         <v>24</v>
       </c>
-      <c r="J60" s="70" t="s">
+      <c r="J63" s="70" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="61" spans="1:10" ht="45">
-      <c r="B61" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="C61" s="49" t="s">
+    <row r="64" spans="1:10" ht="45">
+      <c r="B64" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="C64" s="49" t="s">
         <v>20</v>
       </c>
-      <c r="D61" s="20"/>
-      <c r="E61" s="21">
+      <c r="D64" s="20"/>
+      <c r="E64" s="21">
         <v>42749</v>
       </c>
-      <c r="F61" s="22" t="s">
+      <c r="F64" s="22" t="s">
         <v>107</v>
       </c>
-      <c r="G61" s="20"/>
-      <c r="H61" s="24" t="s">
+      <c r="G64" s="20"/>
+      <c r="H64" s="24" t="s">
         <v>69</v>
       </c>
-      <c r="I61" s="24" t="s">
+      <c r="I64" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="J61" s="67"/>
-    </row>
-    <row r="62" spans="1:10" ht="30">
-      <c r="B62" s="34" t="s">
-        <v>16</v>
-      </c>
-      <c r="C62" s="50" t="s">
+      <c r="J64" s="67"/>
+    </row>
+    <row r="65" spans="2:10" ht="30">
+      <c r="B65" s="34" t="s">
+        <v>16</v>
+      </c>
+      <c r="C65" s="50" t="s">
         <v>20</v>
       </c>
-      <c r="D62" s="35"/>
-      <c r="E62" s="36">
+      <c r="D65" s="35"/>
+      <c r="E65" s="36">
         <v>42809</v>
       </c>
-      <c r="F62" s="37" t="s">
+      <c r="F65" s="37" t="s">
         <v>97</v>
       </c>
-      <c r="G62" s="40"/>
-      <c r="H62" s="38" t="s">
+      <c r="G65" s="40"/>
+      <c r="H65" s="38" t="s">
         <v>154</v>
       </c>
-      <c r="I62" s="38" t="s">
+      <c r="I65" s="38" t="s">
         <v>155</v>
       </c>
-      <c r="J62" s="66"/>
-    </row>
-    <row r="64" spans="1:10" ht="28.5" customHeight="1">
-      <c r="B64" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="C64" s="54" t="s">
+      <c r="J65" s="66"/>
+    </row>
+    <row r="67" spans="2:10" ht="28.5" customHeight="1">
+      <c r="B67" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C67" s="54" t="s">
         <v>176</v>
       </c>
-      <c r="D64" s="14" t="s">
+      <c r="D67" s="14" t="s">
         <v>133</v>
       </c>
-      <c r="E64" s="18">
+      <c r="E67" s="18">
         <v>42781</v>
       </c>
-      <c r="F64" s="13" t="s">
+      <c r="F67" s="13" t="s">
         <v>136</v>
       </c>
-      <c r="G64" s="14" t="s">
+      <c r="G67" s="14" t="s">
         <v>134</v>
       </c>
-      <c r="H64" s="15" t="s">
+      <c r="H67" s="15" t="s">
         <v>135</v>
       </c>
-      <c r="I64" s="14"/>
-      <c r="J64" s="69"/>
-    </row>
-    <row r="65" spans="2:10" ht="30">
-      <c r="B65" s="43" t="s">
-        <v>16</v>
-      </c>
-      <c r="C65" s="55" t="s">
+      <c r="I67" s="14"/>
+      <c r="J67" s="69"/>
+    </row>
+    <row r="68" spans="2:10" ht="30">
+      <c r="B68" s="43" t="s">
+        <v>16</v>
+      </c>
+      <c r="C68" s="55" t="s">
         <v>176</v>
       </c>
-      <c r="D65" s="33" t="s">
+      <c r="D68" s="33" t="s">
         <v>177</v>
       </c>
-      <c r="E65" s="44">
+      <c r="E68" s="44">
         <v>42468</v>
       </c>
-      <c r="F65" s="45" t="s">
+      <c r="F68" s="45" t="s">
         <v>136</v>
       </c>
-      <c r="G65" s="46" t="s">
+      <c r="G68" s="46" t="s">
         <v>186</v>
       </c>
-      <c r="H65" s="47" t="s">
+      <c r="H68" s="47" t="s">
         <v>178</v>
       </c>
-      <c r="I65" s="47"/>
-      <c r="J65" s="70"/>
-    </row>
-    <row r="66" spans="2:10" ht="30">
-      <c r="B66" s="43" t="s">
-        <v>16</v>
-      </c>
-      <c r="C66" s="55" t="s">
+      <c r="I68" s="47"/>
+      <c r="J68" s="70"/>
+    </row>
+    <row r="69" spans="2:10" ht="30">
+      <c r="B69" s="43" t="s">
+        <v>16</v>
+      </c>
+      <c r="C69" s="55" t="s">
         <v>176</v>
       </c>
-      <c r="D66" s="33" t="s">
+      <c r="D69" s="33" t="s">
         <v>179</v>
       </c>
-      <c r="E66" s="44">
+      <c r="E69" s="44">
         <v>42451</v>
       </c>
-      <c r="F66" s="45" t="s">
+      <c r="F69" s="45" t="s">
         <v>136</v>
       </c>
-      <c r="G66" s="46" t="s">
+      <c r="G69" s="46" t="s">
         <v>185</v>
       </c>
-      <c r="H66" s="47" t="s">
+      <c r="H69" s="47" t="s">
         <v>180</v>
       </c>
-      <c r="I66" s="47"/>
-      <c r="J66" s="70"/>
-    </row>
-    <row r="67" spans="2:10" ht="45">
-      <c r="B67" s="43" t="s">
-        <v>16</v>
-      </c>
-      <c r="C67" s="55" t="s">
+      <c r="I69" s="47"/>
+      <c r="J69" s="70"/>
+    </row>
+    <row r="70" spans="2:10" ht="45">
+      <c r="B70" s="43" t="s">
+        <v>16</v>
+      </c>
+      <c r="C70" s="55" t="s">
         <v>176</v>
       </c>
-      <c r="D67" s="33" t="s">
+      <c r="D70" s="33" t="s">
         <v>181</v>
       </c>
-      <c r="E67" s="44">
+      <c r="E70" s="44">
         <v>42488</v>
       </c>
-      <c r="F67" s="45" t="s">
+      <c r="F70" s="45" t="s">
         <v>136</v>
       </c>
-      <c r="G67" s="46" t="s">
+      <c r="G70" s="46" t="s">
         <v>184</v>
       </c>
-      <c r="H67" s="47" t="s">
+      <c r="H70" s="47" t="s">
         <v>182</v>
       </c>
-      <c r="I67" s="47" t="s">
+      <c r="I70" s="47" t="s">
         <v>183</v>
       </c>
-      <c r="J67" s="70"/>
-    </row>
-    <row r="68" spans="2:10" ht="30">
-      <c r="B68" s="26" t="s">
-        <v>16</v>
-      </c>
-      <c r="C68" s="51" t="s">
+      <c r="J70" s="70"/>
+    </row>
+    <row r="71" spans="2:10" ht="30">
+      <c r="B71" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="C71" s="51" t="s">
         <v>176</v>
       </c>
-      <c r="D68" s="27" t="s">
+      <c r="D71" s="27" t="s">
         <v>181</v>
       </c>
-      <c r="E68" s="28">
+      <c r="E71" s="28">
         <v>43013</v>
       </c>
-      <c r="F68" s="29" t="s">
+      <c r="F71" s="29" t="s">
         <v>98</v>
       </c>
-      <c r="G68" s="30" t="s">
+      <c r="G71" s="30" t="s">
         <v>246</v>
       </c>
-      <c r="H68" s="31" t="s">
+      <c r="H71" s="31" t="s">
         <v>224</v>
       </c>
-      <c r="I68" s="31" t="s">
+      <c r="I71" s="31" t="s">
         <v>225</v>
       </c>
-      <c r="J68" s="68"/>
-    </row>
-    <row r="69" spans="2:10" ht="30">
-      <c r="B69" s="26" t="s">
-        <v>16</v>
-      </c>
-      <c r="C69" s="51" t="s">
+      <c r="J71" s="68"/>
+    </row>
+    <row r="72" spans="2:10" ht="30">
+      <c r="B72" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="C72" s="51" t="s">
         <v>176</v>
       </c>
-      <c r="D69" s="27" t="s">
+      <c r="D72" s="27" t="s">
         <v>181</v>
       </c>
-      <c r="E69" s="28">
+      <c r="E72" s="28">
         <v>43047</v>
       </c>
-      <c r="F69" s="29" t="s">
+      <c r="F72" s="29" t="s">
         <v>98</v>
       </c>
-      <c r="G69" s="30" t="s">
+      <c r="G72" s="30" t="s">
         <v>247</v>
       </c>
-      <c r="H69" s="31" t="s">
+      <c r="H72" s="31" t="s">
         <v>248</v>
       </c>
-      <c r="I69" s="31" t="s">
+      <c r="I72" s="31" t="s">
         <v>249</v>
       </c>
-      <c r="J69" s="68"/>
+      <c r="J72" s="68"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3317,17 +3434,17 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:13" ht="21">
-      <c r="B2" s="116" t="s">
+      <c r="B2" s="117" t="s">
         <v>138</v>
       </c>
-      <c r="C2" s="116"/>
-      <c r="D2" s="116"/>
-      <c r="E2" s="116"/>
-      <c r="F2" s="116"/>
-      <c r="G2" s="116"/>
-      <c r="H2" s="116"/>
-      <c r="I2" s="116"/>
-      <c r="J2" s="116"/>
+      <c r="C2" s="117"/>
+      <c r="D2" s="117"/>
+      <c r="E2" s="117"/>
+      <c r="F2" s="117"/>
+      <c r="G2" s="117"/>
+      <c r="H2" s="117"/>
+      <c r="I2" s="117"/>
+      <c r="J2" s="117"/>
     </row>
     <row r="4" spans="2:13" s="8" customFormat="1">
       <c r="B4" s="3" t="s">

</xml_diff>